<commit_message>
Updated, audio should work but might need to change when changing branch
</commit_message>
<xml_diff>
--- a/hmoob_lus/PDF HLLA.xlsx
+++ b/hmoob_lus/PDF HLLA.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ntxhw\Desktop\Projects\HLLA\hmoob_lus\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02873C97-7049-4087-AB12-80D6D8A91B5A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D66245D4-2CCF-4207-9A14-3DA3BEF2B359}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -61,10 +61,10 @@
     <t>Animals</t>
   </si>
   <si>
-    <t>/localhost:8000/media/Male%20-%20Cat.wav</t>
-  </si>
-  <si>
-    <t>/localhost:8000/media/Female%20-%20Cat.wav</t>
+    <t>https://raw.githubusercontent.com/xvang3/HLLA/sqlite-testing/hmoob_lus/media/Male%20-%20Cat.wav</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/xvang3/HLLA/sqlite-testing/hmoob_lus/media/Female%20-%20Cat.wav</t>
   </si>
   <si>
     <t>dog</t>
@@ -73,10 +73,10 @@
     <t>dev/aub</t>
   </si>
   <si>
-    <t>/localhost:8000/media/Male%20-%20Dog%201.wav</t>
-  </si>
-  <si>
-    <t>/localhost:8000/media/Female%20-%20Dog%201.wav</t>
+    <t>https://raw.githubusercontent.com/xvang3/HLLA/sqlite-testing/hmoob_lus/media/Male%20-%20Dog%201.wav</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/xvang3/HLLA/sqlite-testing/hmoob_lus/media/Female%20-%20Dog%201.wav</t>
   </si>
   <si>
     <t>cow</t>
@@ -85,10 +85,10 @@
     <t>nyuj</t>
   </si>
   <si>
-    <t>/localhost:8000/media/Male%20-%20Cow.wav</t>
-  </si>
-  <si>
-    <t>/localhost:8000/media/Female%20-%20Cow.wav</t>
+    <t>https://raw.githubusercontent.com/xvang3/HLLA/sqlite-testing/hmoob_lus/media/Male%20-%20Cow.wav</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/xvang3/HLLA/sqlite-testing/hmoob_lus/media/Female%20-%20Cow.wav</t>
   </si>
   <si>
     <t>pig</t>
@@ -97,10 +97,10 @@
     <t>npua</t>
   </si>
   <si>
-    <t>/localhost:8000/media/Male%20-%20Pig.wav</t>
-  </si>
-  <si>
-    <t>/localhost:8000/media/Female%20-%20Pig.wav</t>
+    <t>https://raw.githubusercontent.com/xvang3/HLLA/sqlite-testing/hmoob_lus/media/Male%20-%20Pig.wav</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/xvang3/HLLA/sqlite-testing/hmoob_lus/media/Female%20-%20Pig.wav</t>
   </si>
   <si>
     <t>chicken</t>
@@ -109,10 +109,10 @@
     <t>qaib</t>
   </si>
   <si>
-    <t>/localhost:8000/media/Male%20-%20Chicken.wav</t>
-  </si>
-  <si>
-    <t>/localhost:8000/media/Female%20-%20Chicken.wav</t>
+    <t>https://raw.githubusercontent.com/xvang3/HLLA/sqlite-testing/hmoob_lus/media/Male%20-%20Chicken.wav</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/xvang3/HLLA/sqlite-testing/hmoob_lus/media/Female%20-%20Chicken.wav</t>
   </si>
   <si>
     <t>zero</t>
@@ -124,10 +124,10 @@
     <t>Numbers</t>
   </si>
   <si>
-    <t>/localhost:8000/media/Male%20-%20Zero.wav</t>
-  </si>
-  <si>
-    <t>/localhost:8000/media/Female%20-%20Zero.wav</t>
+    <t>https://raw.githubusercontent.com/xvang3/HLLA/sqlite-testing/hmoob_lus/media/Male%20-%20Zero.wav</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/xvang3/HLLA/sqlite-testing/hmoob_lus/media/Female%20-%20Zero.wav</t>
   </si>
   <si>
     <t>one</t>
@@ -136,10 +136,10 @@
     <t>ib</t>
   </si>
   <si>
-    <t>/localhost:8000/media/Male%20-%20One.wav</t>
-  </si>
-  <si>
-    <t>/localhost:8000/media/Female%20-%20One.wav</t>
+    <t>https://raw.githubusercontent.com/xvang3/HLLA/sqlite-testing/hmoob_lus/media/Male%20-%20One.wav</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/xvang3/HLLA/sqlite-testing/hmoob_lus/media/Female%20-%20One.wav</t>
   </si>
   <si>
     <t>two</t>
@@ -148,10 +148,10 @@
     <t>ob</t>
   </si>
   <si>
-    <t>/localhost:8000/media/Male%20-%20Two.wav</t>
-  </si>
-  <si>
-    <t>/localhost:8000/media/Female%20-%20Two.wav</t>
+    <t>https://raw.githubusercontent.com/xvang3/HLLA/sqlite-testing/hmoob_lus/media/Male%20-%20Two.wav</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/xvang3/HLLA/sqlite-testing/hmoob_lus/media/Female%20-%20Two.wav</t>
   </si>
   <si>
     <t>three</t>
@@ -160,10 +160,10 @@
     <t>peb</t>
   </si>
   <si>
-    <t>/localhost:8000/media/Male%20-%20Three.wav</t>
-  </si>
-  <si>
-    <t>/localhost:8000/media/Female%20-%20Three.wav</t>
+    <t>https://raw.githubusercontent.com/xvang3/HLLA/sqlite-testing/hmoob_lus/media/Male%20-%20Three.wav</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/xvang3/HLLA/sqlite-testing/hmoob_lus/media/Female%20-%20Three.wav</t>
   </si>
   <si>
     <t>four</t>
@@ -172,10 +172,10 @@
     <t>plaub</t>
   </si>
   <si>
-    <t>/localhost:8000/media/Male%20-%20Four.wav</t>
-  </si>
-  <si>
-    <t>/localhost:8000/media/Female%20-%20Four.wav</t>
+    <t>https://raw.githubusercontent.com/xvang3/HLLA/sqlite-testing/hmoob_lus/media/Male%20-%20Four.wav</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/xvang3/HLLA/sqlite-testing/hmoob_lus/media/Female%20-%20Four.wav</t>
   </si>
   <si>
     <t>five</t>
@@ -184,10 +184,10 @@
     <t>tsib</t>
   </si>
   <si>
-    <t>/localhost:8000/media/Male%20-%20Five.wav</t>
-  </si>
-  <si>
-    <t>/localhost:8000/media/Female%20-%20Five.wav</t>
+    <t>https://raw.githubusercontent.com/xvang3/HLLA/sqlite-testing/hmoob_lus/media/Male%20-%20Five.wav</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/xvang3/HLLA/sqlite-testing/hmoob_lus/media/Female%20-%20Five.wav</t>
   </si>
   <si>
     <t>six</t>
@@ -196,10 +196,10 @@
     <t>rau</t>
   </si>
   <si>
-    <t>/localhost:8000/media/Male%20-%20Six.wav</t>
-  </si>
-  <si>
-    <t>/localhost:8000/media/Female%20-%20Six.wav</t>
+    <t>https://raw.githubusercontent.com/xvang3/HLLA/sqlite-testing/hmoob_lus/media/Male%20-%20Six.wav</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/xvang3/HLLA/sqlite-testing/hmoob_lus/media/Female%20-%20Six.wav</t>
   </si>
   <si>
     <t>seven</t>
@@ -208,10 +208,10 @@
     <t>xya</t>
   </si>
   <si>
-    <t>/localhost:8000/media/Male%20-%20Seven.wav</t>
-  </si>
-  <si>
-    <t>/localhost:8000/media/Female%20-%20Seven.wav</t>
+    <t>https://raw.githubusercontent.com/xvang3/HLLA/sqlite-testing/hmoob_lus/media/Male%20-%20Seven.wav</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/xvang3/HLLA/sqlite-testing/hmoob_lus/media/Female%20-%20Seven.wav</t>
   </si>
   <si>
     <t>eight</t>
@@ -220,10 +220,10 @@
     <t>yim</t>
   </si>
   <si>
-    <t>/localhost:8000/media/Male%20-%20Eight.wav</t>
-  </si>
-  <si>
-    <t>/localhost:8000/media/Female%20-%20Eight.wav</t>
+    <t>https://raw.githubusercontent.com/xvang3/HLLA/sqlite-testing/hmoob_lus/media/Male%20-%20Eight.wav</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/xvang3/HLLA/sqlite-testing/hmoob_lus/media/Female%20-%20Eight.wav</t>
   </si>
   <si>
     <t>nine</t>
@@ -232,10 +232,10 @@
     <t>cuaj</t>
   </si>
   <si>
-    <t>/localhost:8000/media/Male%20-%20Nine.wav</t>
-  </si>
-  <si>
-    <t>/localhost:8000/media/Female%20-%20Nine.wav</t>
+    <t>https://raw.githubusercontent.com/xvang3/HLLA/sqlite-testing/hmoob_lus/media/Male%20-%20Nine.wav</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/xvang3/HLLA/sqlite-testing/hmoob_lus/media/Female%20-%20Nine.wav</t>
   </si>
   <si>
     <t>ten</t>
@@ -244,10 +244,10 @@
     <t>kaum</t>
   </si>
   <si>
-    <t>/localhost:8000/media/Male%20-%20Ten.wav</t>
-  </si>
-  <si>
-    <t>/localhost:8000/media/Female%20-%20Ten.wav</t>
+    <t>https://raw.githubusercontent.com/xvang3/HLLA/sqlite-testing/hmoob_lus/media/Male%20-%20Ten.wav</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/xvang3/HLLA/sqlite-testing/hmoob_lus/media/Female%20-%20Ten.wav</t>
   </si>
   <si>
     <t>hello</t>
@@ -259,10 +259,10 @@
     <t>Common Phrases</t>
   </si>
   <si>
-    <t>/localhost:8000/media/Male%20-%20Hello.wav</t>
-  </si>
-  <si>
-    <t>/localhost:8000/media/Female%20-%20Hello.wav</t>
+    <t>https://raw.githubusercontent.com/xvang3/HLLA/sqlite-testing/hmoob_lus/media/Male%20-%20Hello.wav</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/xvang3/HLLA/sqlite-testing/hmoob_lus/media/Female%20-%20Hello.wav</t>
   </si>
   <si>
     <t>goodbye</t>
@@ -271,10 +271,10 @@
     <t>sib ntsib dua</t>
   </si>
   <si>
-    <t>/localhost:8000/media/Male%20-%20Goodbye%20(See%20you%20again).wav</t>
-  </si>
-  <si>
-    <t>/localhost:8000/media/Female%20-%20Goodbye%20(See%20you%20again).wav</t>
+    <t>https://raw.githubusercontent.com/xvang3/HLLA/sqlite-testing/hmoob_lus/media/Male%20-%20Goodbye%20(See%20you%20again).wav</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/xvang3/HLLA/sqlite-testing/hmoob_lus/media/Female%20-%20Goodbye%20(See%20you%20again).wav</t>
   </si>
   <si>
     <t>my name is</t>
@@ -283,10 +283,10 @@
     <t>kuv lub npe yog</t>
   </si>
   <si>
-    <t>/localhost:8000/media/Male%20-%20My%20name%20is.wav</t>
-  </si>
-  <si>
-    <t>/localhost:8000/media/Female%20-%20My%20name%20is.wav</t>
+    <t>https://raw.githubusercontent.com/xvang3/HLLA/sqlite-testing/hmoob_lus/media/Male%20-%20My%20name%20is.wav</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/xvang3/HLLA/sqlite-testing/hmoob_lus/media/Female%20-%20My%20name%20is.wav</t>
   </si>
   <si>
     <t>thank you</t>
@@ -295,10 +295,10 @@
     <t>ua tsaug</t>
   </si>
   <si>
-    <t>/localhost:8000/media/Male%20-%20Thank%20you.wav</t>
-  </si>
-  <si>
-    <t>/localhost:8000/media/Female%20-%20Thank%20you.wav</t>
+    <t>https://raw.githubusercontent.com/xvang3/HLLA/sqlite-testing/hmoob_lus/media/Male%20-%20Thank%20you.wav</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/xvang3/HLLA/sqlite-testing/hmoob_lus/media/Female%20-%20Thank%20you.wav</t>
   </si>
   <si>
     <t>mother</t>
@@ -310,10 +310,10 @@
     <t>Family</t>
   </si>
   <si>
-    <t>/localhost:8000/media/Male%20-%20Mom.wav</t>
-  </si>
-  <si>
-    <t>/localhost:8000/media/Female%20-%20Mom.wav</t>
+    <t>https://raw.githubusercontent.com/xvang3/HLLA/sqlite-testing/hmoob_lus/media/Male%20-%20Mom.wav</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/xvang3/HLLA/sqlite-testing/hmoob_lus/media/Female%20-%20Mom.wav</t>
   </si>
   <si>
     <t>father</t>
@@ -322,10 +322,10 @@
     <t>txiv</t>
   </si>
   <si>
-    <t>/localhost:8000/media/Male%20-%20Dad.wav</t>
-  </si>
-  <si>
-    <t>/localhost:8000/media/Female%20-%20Dad.wav</t>
+    <t>https://raw.githubusercontent.com/xvang3/HLLA/sqlite-testing/hmoob_lus/media/Male%20-%20Dad.wav</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/xvang3/HLLA/sqlite-testing/hmoob_lus/media/Female%20-%20Dad.wav</t>
   </si>
   <si>
     <t>older brother (female use)</t>
@@ -334,7 +334,7 @@
     <t>nus hlob</t>
   </si>
   <si>
-    <t>/localhost:8000/media/Female%20-%20Older%20Brother.wav</t>
+    <t>https://raw.githubusercontent.com/xvang3/HLLA/sqlite-testing/hmoob_lus/media/Female%20-%20Older%20Brother.wav</t>
   </si>
   <si>
     <t>younger brother (female use)</t>
@@ -343,7 +343,7 @@
     <t>nus yaus</t>
   </si>
   <si>
-    <t>/localhost:8000/media/Female%20-%20Younger%20Brother.wav</t>
+    <t>https://raw.githubusercontent.com/xvang3/HLLA/sqlite-testing/hmoob_lus/media/Female%20-%20Younger%20Brother.wav</t>
   </si>
   <si>
     <t>older sister (female use)</t>
@@ -352,7 +352,7 @@
     <t>niam laus</t>
   </si>
   <si>
-    <t>/localhost:8000/media/Female%20-%20Older%20Sister.wav</t>
+    <t>https://raw.githubusercontent.com/xvang3/HLLA/sqlite-testing/hmoob_lus/media/Female%20-%20Older%20Sister.wav</t>
   </si>
   <si>
     <t>younger sister (female use)</t>
@@ -361,7 +361,7 @@
     <t>niam hluas</t>
   </si>
   <si>
-    <t>/localhost:8000/media/Female%20-%20Younger%20Sister.wav</t>
+    <t>https://raw.githubusercontent.com/xvang3/HLLA/sqlite-testing/hmoob_lus/media/Female%20-%20Younger%20Sister.wav</t>
   </si>
   <si>
     <t>older brother (male use)</t>
@@ -370,7 +370,7 @@
     <t>tij lauj</t>
   </si>
   <si>
-    <t>/localhost:8000/media/Male%20-%20Older%20Brother.wav</t>
+    <t>https://raw.githubusercontent.com/xvang3/HLLA/sqlite-testing/hmoob_lus/media/Male%20-%20Older%20Brother.wav</t>
   </si>
   <si>
     <t>younger brother (male use)</t>
@@ -379,7 +379,7 @@
     <t>kwv</t>
   </si>
   <si>
-    <t>/localhost:8000/media/Male%20-%20Younger%20Brother.wav</t>
+    <t>https://raw.githubusercontent.com/xvang3/HLLA/sqlite-testing/hmoob_lus/media/Male%20-%20Younger%20Brother.wav</t>
   </si>
   <si>
     <t>older sister (male use)</t>
@@ -388,7 +388,7 @@
     <t>muam hlob</t>
   </si>
   <si>
-    <t>/localhost:8000/media/Male%20-%20Older%20Sister.wav</t>
+    <t>https://raw.githubusercontent.com/xvang3/HLLA/sqlite-testing/hmoob_lus/media/Male%20-%20Older%20Sister.wav</t>
   </si>
   <si>
     <t>younger sister (male use)</t>
@@ -397,7 +397,7 @@
     <t>muam yaus</t>
   </si>
   <si>
-    <t>/localhost:8000/media/Male%20-%20Younger%20Sister.wav</t>
+    <t>https://raw.githubusercontent.com/xvang3/HLLA/sqlite-testing/hmoob_lus/media/Male%20-%20Younger%20Sister.wav</t>
   </si>
   <si>
     <t>grandmother (maternal)</t>
@@ -406,10 +406,10 @@
     <t>niam tais</t>
   </si>
   <si>
-    <t>/localhost:8000/media/Male%20-%20Maternal%20Auntie%20or%20Grandmother.wav</t>
-  </si>
-  <si>
-    <t>/localhost:8000/media/Female%20-%20Maternal%20Auntie%20or%20Grandmother.wav</t>
+    <t>https://raw.githubusercontent.com/xvang3/HLLA/sqlite-testing/hmoob_lus/media/Male%20-%20Maternal%20Auntie%20or%20Grandmother.wav</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/xvang3/HLLA/sqlite-testing/hmoob_lus/media/Female%20-%20Maternal%20Auntie%20or%20Grandmother.wav</t>
   </si>
   <si>
     <t>grandfather (maternal)</t>
@@ -418,10 +418,10 @@
     <t>yawm txiv</t>
   </si>
   <si>
-    <t>/localhost:8000/media/Male%20-%20Maternal%20Grandfather.wav</t>
-  </si>
-  <si>
-    <t>/localhost:8000/media/Female%20-%20Maternal%20Grandfather.wav</t>
+    <t>https://raw.githubusercontent.com/xvang3/HLLA/sqlite-testing/hmoob_lus/media/Male%20-%20Maternal%20Grandfather.wav</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/xvang3/HLLA/sqlite-testing/hmoob_lus/media/Female%20-%20Maternal%20Grandfather.wav</t>
   </si>
   <si>
     <t>grandmother (paternal)</t>
@@ -430,10 +430,10 @@
     <t>niam pog</t>
   </si>
   <si>
-    <t>/localhost:8000/media/Male%20-%20Paternal%20Grandmother.wav</t>
-  </si>
-  <si>
-    <t>/localhost:8000/media/Female%20-%20Paternal%20Grandmother.wav</t>
+    <t>https://raw.githubusercontent.com/xvang3/HLLA/sqlite-testing/hmoob_lus/media/Male%20-%20Paternal%20Grandmother.wav</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/xvang3/HLLA/sqlite-testing/hmoob_lus/media/Female%20-%20Paternal%20Grandmother.wav</t>
   </si>
   <si>
     <t>grandfather (paternal)</t>
@@ -442,10 +442,10 @@
     <t>txiv yawg</t>
   </si>
   <si>
-    <t>/localhost:8000/media/Male%20-%20Paternal%20Grandfather.wav</t>
-  </si>
-  <si>
-    <t>/localhost:8000/media/Female%20-%20Paternal%20Grandfather.wav</t>
+    <t>https://raw.githubusercontent.com/xvang3/HLLA/sqlite-testing/hmoob_lus/media/Male%20-%20Paternal%20Grandfather.wav</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/xvang3/HLLA/sqlite-testing/hmoob_lus/media/Female%20-%20Paternal%20Grandfather.wav</t>
   </si>
 </sst>
 </file>
@@ -811,7 +811,7 @@
   <dimension ref="A1:J35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -819,8 +819,8 @@
     <col min="1" max="1" width="25.6328125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.90625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="15.453125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="74.08984375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="76" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="125.1796875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="127" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="18.08984375" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="9.6328125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="14.36328125" bestFit="1" customWidth="1"/>

</xml_diff>

<commit_message>
Recorded and added male audio
</commit_message>
<xml_diff>
--- a/hmoob_lus/PDF HLLA.xlsx
+++ b/hmoob_lus/PDF HLLA.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\logao\OneDrive\Documents\Desktop\HLLA\hmoob_lus\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ntxhw\Desktop\Projects\HLLA\hmoob_lus\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A41E0DE8-CCDF-41AE-B750-70E8A99BF2DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BED1C94-1FA9-477C-BBE5-52C42723C5C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14625" windowHeight="12863" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="324" uniqueCount="254">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="362" uniqueCount="292">
   <si>
     <t>English Word</t>
   </si>
@@ -787,6 +787,120 @@
   </si>
   <si>
     <t>(-)/no tone</t>
+  </si>
+  <si>
+    <t>Male – Tone Marker B.wav</t>
+  </si>
+  <si>
+    <t>Male – Tone Marker J.wav</t>
+  </si>
+  <si>
+    <t>Male – Tone Marker V.wav</t>
+  </si>
+  <si>
+    <t>Male – Tone Marker S.wav</t>
+  </si>
+  <si>
+    <t>Male – Tone Marker G.wav</t>
+  </si>
+  <si>
+    <t>Male – Tone Marker M.wav</t>
+  </si>
+  <si>
+    <t>Male – Tone Marker D.wav</t>
+  </si>
+  <si>
+    <t>Male – Tone Marker (-).wav</t>
+  </si>
+  <si>
+    <t>Male – Single Vowel A.wav</t>
+  </si>
+  <si>
+    <t>Male – Single Vowel E.wav</t>
+  </si>
+  <si>
+    <t>Male – Single Vowel I.wav</t>
+  </si>
+  <si>
+    <t>Male – Single Vowel O.wav</t>
+  </si>
+  <si>
+    <t>Male – Single Vowel U.wav</t>
+  </si>
+  <si>
+    <t>Male – Single Vowel W.wav</t>
+  </si>
+  <si>
+    <t>Male – Double Vowel AI.wav</t>
+  </si>
+  <si>
+    <t>Male – Double Vowel AU.wav</t>
+  </si>
+  <si>
+    <t>Male – Double Vowel AW.wav</t>
+  </si>
+  <si>
+    <t>Male – Double Vowel EE.wav</t>
+  </si>
+  <si>
+    <t>Male – Double Vowel IA.wav</t>
+  </si>
+  <si>
+    <t>Male – Double Vowel OO.wav</t>
+  </si>
+  <si>
+    <t>Male – Double Vowel UA.wav</t>
+  </si>
+  <si>
+    <t>Male – Consonant C.wav</t>
+  </si>
+  <si>
+    <t>Male – Consonant D.wav</t>
+  </si>
+  <si>
+    <t>Male – Consonant F.wav</t>
+  </si>
+  <si>
+    <t>Male – Consonant H.wav</t>
+  </si>
+  <si>
+    <t>Male – Consonant K.wav</t>
+  </si>
+  <si>
+    <t>Male – Consonant L.wav</t>
+  </si>
+  <si>
+    <t>Male – Consonant M.wav</t>
+  </si>
+  <si>
+    <t>Male – Consonant N.wav</t>
+  </si>
+  <si>
+    <t>Male – Consonant P.wav</t>
+  </si>
+  <si>
+    <t>Male – Consonant Q.wav</t>
+  </si>
+  <si>
+    <t>Male – Consonant R.wav</t>
+  </si>
+  <si>
+    <t>Male – Consonant S.wav</t>
+  </si>
+  <si>
+    <t>Male – Consonant T.wav</t>
+  </si>
+  <si>
+    <t>Male – Consonant V.wav</t>
+  </si>
+  <si>
+    <t>Male – Consonant X.wav</t>
+  </si>
+  <si>
+    <t>Male – Consonant Y.wav</t>
+  </si>
+  <si>
+    <t>Male – Consonant Z.wav</t>
   </si>
 </sst>
 </file>
@@ -867,14 +981,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -1097,26 +1210,26 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A63" zoomScale="63" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D40" sqref="D40"/>
+    <sheetView tabSelected="1" topLeftCell="A51" zoomScale="63" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D33" sqref="D33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.3984375" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultColWidth="14.36328125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="25.53125" customWidth="1"/>
-    <col min="2" max="2" width="13.86328125" customWidth="1"/>
-    <col min="3" max="3" width="15.3984375" customWidth="1"/>
-    <col min="4" max="4" width="125.1328125" customWidth="1"/>
+    <col min="1" max="1" width="25.54296875" customWidth="1"/>
+    <col min="2" max="2" width="13.81640625" customWidth="1"/>
+    <col min="3" max="3" width="15.36328125" customWidth="1"/>
+    <col min="4" max="4" width="125.08984375" customWidth="1"/>
     <col min="5" max="5" width="127" customWidth="1"/>
-    <col min="6" max="6" width="18.1328125" customWidth="1"/>
-    <col min="7" max="7" width="9.53125" customWidth="1"/>
-    <col min="8" max="8" width="14.3984375" customWidth="1"/>
-    <col min="9" max="9" width="14.1328125" customWidth="1"/>
-    <col min="10" max="10" width="15.86328125" customWidth="1"/>
-    <col min="11" max="26" width="8.73046875" customWidth="1"/>
+    <col min="6" max="6" width="18.08984375" customWidth="1"/>
+    <col min="7" max="7" width="9.54296875" customWidth="1"/>
+    <col min="8" max="8" width="14.36328125" customWidth="1"/>
+    <col min="9" max="9" width="14.08984375" customWidth="1"/>
+    <col min="10" max="10" width="15.81640625" customWidth="1"/>
+    <col min="11" max="26" width="8.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1148,7 +1261,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>10</v>
       </c>
@@ -1165,7 +1278,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>15</v>
       </c>
@@ -1182,7 +1295,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
         <v>19</v>
       </c>
@@ -1199,7 +1312,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
         <v>23</v>
       </c>
@@ -1216,7 +1329,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
         <v>27</v>
       </c>
@@ -1233,7 +1346,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="7" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="2" t="s">
         <v>31</v>
       </c>
@@ -1250,7 +1363,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="8" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="2" t="s">
         <v>36</v>
       </c>
@@ -1267,7 +1380,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="9" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="2" t="s">
         <v>40</v>
       </c>
@@ -1284,7 +1397,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="2" t="s">
         <v>44</v>
       </c>
@@ -1301,7 +1414,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="11" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" s="2" t="s">
         <v>48</v>
       </c>
@@ -1318,7 +1431,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="12" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" s="2" t="s">
         <v>52</v>
       </c>
@@ -1335,7 +1448,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="13" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="2" t="s">
         <v>56</v>
       </c>
@@ -1352,7 +1465,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="14" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" s="2" t="s">
         <v>60</v>
       </c>
@@ -1369,7 +1482,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="15" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15" s="2" t="s">
         <v>64</v>
       </c>
@@ -1386,7 +1499,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="16" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A16" s="2" t="s">
         <v>68</v>
       </c>
@@ -1403,7 +1516,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="17" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A17" s="2" t="s">
         <v>72</v>
       </c>
@@ -1420,7 +1533,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="18" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A18" s="2" t="s">
         <v>76</v>
       </c>
@@ -1437,7 +1550,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="19" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A19" s="2" t="s">
         <v>81</v>
       </c>
@@ -1454,7 +1567,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="20" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A20" s="2" t="s">
         <v>85</v>
       </c>
@@ -1471,7 +1584,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="21" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A21" s="2" t="s">
         <v>89</v>
       </c>
@@ -1488,7 +1601,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="22" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A22" s="2" t="s">
         <v>93</v>
       </c>
@@ -1505,7 +1618,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="23" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A23" s="2" t="s">
         <v>98</v>
       </c>
@@ -1522,7 +1635,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="24" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A24" s="2" t="s">
         <v>102</v>
       </c>
@@ -1536,7 +1649,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="25" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A25" s="2" t="s">
         <v>105</v>
       </c>
@@ -1550,7 +1663,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="26" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A26" s="2" t="s">
         <v>108</v>
       </c>
@@ -1564,7 +1677,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="27" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A27" s="2" t="s">
         <v>111</v>
       </c>
@@ -1578,7 +1691,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="28" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A28" s="2" t="s">
         <v>114</v>
       </c>
@@ -1592,7 +1705,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="29" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A29" s="2" t="s">
         <v>117</v>
       </c>
@@ -1606,7 +1719,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="30" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A30" s="2" t="s">
         <v>120</v>
       </c>
@@ -1620,7 +1733,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="31" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A31" s="2" t="s">
         <v>123</v>
       </c>
@@ -1634,7 +1747,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="32" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A32" s="2" t="s">
         <v>126</v>
       </c>
@@ -1651,7 +1764,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="33" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A33" s="2" t="s">
         <v>130</v>
       </c>
@@ -1668,7 +1781,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="34" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A34" s="2" t="s">
         <v>134</v>
       </c>
@@ -1685,7 +1798,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="35" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A35" s="2" t="s">
         <v>138</v>
       </c>
@@ -1702,1465 +1815,1579 @@
         <v>141</v>
       </c>
     </row>
-    <row r="36" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A36" s="4" t="s">
+    <row r="36" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A36" t="s">
         <v>142</v>
       </c>
-      <c r="B36" s="4" t="s">
+      <c r="B36" t="s">
         <v>148</v>
       </c>
-      <c r="C36" s="4" t="s">
+      <c r="C36" t="s">
         <v>157</v>
       </c>
-      <c r="E36" s="5" t="s">
+      <c r="D36" t="s">
+        <v>254</v>
+      </c>
+      <c r="E36" s="4" t="s">
         <v>215</v>
       </c>
     </row>
-    <row r="37" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A37" s="4" t="s">
+    <row r="37" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A37" t="s">
         <v>143</v>
       </c>
-      <c r="B37" s="4" t="s">
+      <c r="B37" t="s">
         <v>149</v>
       </c>
-      <c r="C37" s="4" t="s">
+      <c r="C37" t="s">
         <v>157</v>
       </c>
-      <c r="E37" s="5" t="s">
+      <c r="D37" t="s">
+        <v>255</v>
+      </c>
+      <c r="E37" s="4" t="s">
         <v>219</v>
       </c>
     </row>
-    <row r="38" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A38" s="4" t="s">
+    <row r="38" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A38" t="s">
         <v>144</v>
       </c>
-      <c r="B38" s="4" t="s">
+      <c r="B38" t="s">
         <v>150</v>
       </c>
-      <c r="C38" s="4" t="s">
+      <c r="C38" t="s">
         <v>157</v>
       </c>
-      <c r="E38" s="5" t="s">
+      <c r="D38" t="s">
+        <v>256</v>
+      </c>
+      <c r="E38" s="4" t="s">
         <v>220</v>
       </c>
     </row>
-    <row r="39" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A39" s="4" t="s">
+    <row r="39" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A39" t="s">
         <v>145</v>
       </c>
-      <c r="B39" s="4" t="s">
+      <c r="B39" t="s">
         <v>151</v>
       </c>
-      <c r="C39" s="4" t="s">
+      <c r="C39" t="s">
         <v>157</v>
       </c>
-      <c r="E39" s="5" t="s">
+      <c r="D39" t="s">
+        <v>257</v>
+      </c>
+      <c r="E39" s="4" t="s">
         <v>221</v>
       </c>
     </row>
-    <row r="40" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A40" s="4" t="s">
+    <row r="40" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A40" t="s">
         <v>146</v>
       </c>
-      <c r="B40" s="4" t="s">
+      <c r="B40" t="s">
         <v>152</v>
       </c>
-      <c r="C40" s="4" t="s">
+      <c r="C40" t="s">
         <v>157</v>
       </c>
-      <c r="E40" s="5" t="s">
+      <c r="D40" t="s">
+        <v>258</v>
+      </c>
+      <c r="E40" s="4" t="s">
         <v>222</v>
       </c>
     </row>
-    <row r="41" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A41" s="4" t="s">
+    <row r="41" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A41" t="s">
         <v>147</v>
       </c>
-      <c r="B41" s="4" t="s">
+      <c r="B41" t="s">
         <v>153</v>
       </c>
-      <c r="C41" s="4" t="s">
+      <c r="C41" t="s">
         <v>157</v>
       </c>
-      <c r="E41" s="5" t="s">
+      <c r="D41" t="s">
+        <v>259</v>
+      </c>
+      <c r="E41" s="4" t="s">
         <v>223</v>
       </c>
     </row>
-    <row r="42" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A42" s="4" t="s">
+    <row r="42" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A42" t="s">
         <v>155</v>
       </c>
-      <c r="B42" s="4" t="s">
+      <c r="B42" t="s">
         <v>154</v>
       </c>
-      <c r="C42" s="4" t="s">
+      <c r="C42" t="s">
         <v>157</v>
       </c>
-      <c r="E42" s="5" t="s">
+      <c r="D42" t="s">
+        <v>260</v>
+      </c>
+      <c r="E42" s="4" t="s">
         <v>224</v>
       </c>
     </row>
-    <row r="43" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A43" s="7" t="s">
+    <row r="43" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A43" s="6" t="s">
         <v>253</v>
       </c>
-      <c r="B43" s="4" t="s">
+      <c r="B43" t="s">
         <v>156</v>
       </c>
-      <c r="C43" s="4" t="s">
+      <c r="C43" t="s">
         <v>157</v>
       </c>
-      <c r="E43" s="5" t="s">
+      <c r="D43" t="s">
+        <v>261</v>
+      </c>
+      <c r="E43" s="4" t="s">
         <v>225</v>
       </c>
     </row>
-    <row r="44" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A44" s="4" t="s">
+    <row r="44" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A44" t="s">
         <v>158</v>
       </c>
-      <c r="B44" s="4" t="s">
+      <c r="B44" t="s">
         <v>159</v>
       </c>
-      <c r="C44" s="4" t="s">
+      <c r="C44" t="s">
         <v>169</v>
       </c>
-      <c r="E44" s="5" t="s">
+      <c r="D44" t="s">
+        <v>262</v>
+      </c>
+      <c r="E44" s="4" t="s">
         <v>216</v>
       </c>
     </row>
-    <row r="45" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A45" s="4" t="s">
+    <row r="45" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A45" t="s">
         <v>160</v>
       </c>
-      <c r="B45" s="4" t="s">
+      <c r="B45" t="s">
         <v>165</v>
       </c>
-      <c r="C45" s="4" t="s">
+      <c r="C45" t="s">
         <v>169</v>
       </c>
-      <c r="E45" s="5" t="s">
+      <c r="D45" t="s">
+        <v>263</v>
+      </c>
+      <c r="E45" s="4" t="s">
         <v>226</v>
       </c>
     </row>
-    <row r="46" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A46" s="4" t="s">
+    <row r="46" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A46" t="s">
         <v>161</v>
       </c>
-      <c r="B46" s="4" t="s">
+      <c r="B46" t="s">
         <v>166</v>
       </c>
-      <c r="C46" s="4" t="s">
+      <c r="C46" t="s">
         <v>169</v>
       </c>
-      <c r="E46" s="5" t="s">
+      <c r="D46" t="s">
+        <v>264</v>
+      </c>
+      <c r="E46" s="4" t="s">
         <v>227</v>
       </c>
     </row>
-    <row r="47" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A47" s="4" t="s">
+    <row r="47" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A47" t="s">
         <v>162</v>
       </c>
-      <c r="B47" s="4" t="s">
+      <c r="B47" t="s">
         <v>15</v>
       </c>
-      <c r="C47" s="4" t="s">
+      <c r="C47" t="s">
         <v>169</v>
       </c>
-      <c r="E47" s="5" t="s">
+      <c r="D47" t="s">
+        <v>265</v>
+      </c>
+      <c r="E47" s="4" t="s">
         <v>228</v>
       </c>
     </row>
-    <row r="48" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A48" s="4" t="s">
+    <row r="48" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A48" t="s">
         <v>163</v>
       </c>
-      <c r="B48" s="4" t="s">
+      <c r="B48" t="s">
         <v>167</v>
       </c>
-      <c r="C48" s="4" t="s">
+      <c r="C48" t="s">
         <v>169</v>
       </c>
-      <c r="E48" s="5" t="s">
+      <c r="D48" t="s">
+        <v>266</v>
+      </c>
+      <c r="E48" s="4" t="s">
         <v>229</v>
       </c>
     </row>
-    <row r="49" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A49" s="4" t="s">
+    <row r="49" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A49" t="s">
         <v>164</v>
       </c>
-      <c r="B49" s="4" t="s">
+      <c r="B49" t="s">
         <v>168</v>
       </c>
-      <c r="C49" s="4" t="s">
+      <c r="C49" t="s">
         <v>169</v>
       </c>
-      <c r="E49" s="5" t="s">
+      <c r="D49" t="s">
+        <v>267</v>
+      </c>
+      <c r="E49" s="4" t="s">
         <v>230</v>
       </c>
     </row>
-    <row r="50" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A50" s="4" t="s">
+    <row r="50" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A50" t="s">
         <v>170</v>
       </c>
-      <c r="B50" s="4" t="s">
+      <c r="B50" t="s">
         <v>28</v>
       </c>
-      <c r="C50" s="4" t="s">
+      <c r="C50" t="s">
         <v>183</v>
       </c>
-      <c r="E50" s="5" t="s">
+      <c r="D50" t="s">
+        <v>268</v>
+      </c>
+      <c r="E50" s="4" t="s">
         <v>217</v>
       </c>
     </row>
-    <row r="51" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A51" s="4" t="s">
+    <row r="51" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A51" t="s">
         <v>171</v>
       </c>
-      <c r="B51" s="4" t="s">
+      <c r="B51" t="s">
         <v>177</v>
       </c>
-      <c r="C51" s="4" t="s">
+      <c r="C51" t="s">
         <v>183</v>
       </c>
-      <c r="E51" s="5" t="s">
+      <c r="D51" t="s">
+        <v>269</v>
+      </c>
+      <c r="E51" s="4" t="s">
         <v>231</v>
       </c>
     </row>
-    <row r="52" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A52" s="4" t="s">
+    <row r="52" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A52" t="s">
         <v>172</v>
       </c>
-      <c r="B52" s="4" t="s">
+      <c r="B52" t="s">
         <v>178</v>
       </c>
-      <c r="C52" s="4" t="s">
+      <c r="C52" t="s">
         <v>183</v>
       </c>
-      <c r="E52" s="5" t="s">
+      <c r="D52" t="s">
+        <v>270</v>
+      </c>
+      <c r="E52" s="4" t="s">
         <v>236</v>
       </c>
     </row>
-    <row r="53" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A53" s="4" t="s">
+    <row r="53" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A53" t="s">
         <v>173</v>
       </c>
-      <c r="B53" s="4" t="s">
+      <c r="B53" t="s">
         <v>179</v>
       </c>
-      <c r="C53" s="4" t="s">
+      <c r="C53" t="s">
         <v>183</v>
       </c>
-      <c r="E53" s="5" t="s">
+      <c r="D53" t="s">
+        <v>271</v>
+      </c>
+      <c r="E53" s="4" t="s">
         <v>232</v>
       </c>
     </row>
-    <row r="54" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A54" s="4" t="s">
+    <row r="54" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A54" t="s">
         <v>174</v>
       </c>
-      <c r="B54" s="4" t="s">
+      <c r="B54" t="s">
         <v>180</v>
       </c>
-      <c r="C54" s="4" t="s">
+      <c r="C54" t="s">
         <v>183</v>
       </c>
-      <c r="E54" s="5" t="s">
+      <c r="D54" t="s">
+        <v>272</v>
+      </c>
+      <c r="E54" s="4" t="s">
         <v>233</v>
       </c>
     </row>
-    <row r="55" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A55" s="4" t="s">
+    <row r="55" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A55" t="s">
         <v>175</v>
       </c>
-      <c r="B55" s="4" t="s">
+      <c r="B55" t="s">
         <v>181</v>
       </c>
-      <c r="C55" s="4" t="s">
+      <c r="C55" t="s">
         <v>183</v>
       </c>
-      <c r="E55" s="5" t="s">
+      <c r="D55" t="s">
+        <v>273</v>
+      </c>
+      <c r="E55" s="4" t="s">
         <v>234</v>
       </c>
     </row>
-    <row r="56" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A56" s="4" t="s">
+    <row r="56" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A56" t="s">
         <v>176</v>
       </c>
-      <c r="B56" s="4" t="s">
+      <c r="B56" t="s">
         <v>182</v>
       </c>
-      <c r="C56" s="4" t="s">
+      <c r="C56" t="s">
         <v>183</v>
       </c>
-      <c r="E56" s="5" t="s">
+      <c r="D56" t="s">
+        <v>274</v>
+      </c>
+      <c r="E56" s="4" t="s">
         <v>235</v>
       </c>
     </row>
-    <row r="57" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A57" s="4" t="s">
+    <row r="57" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A57" t="s">
         <v>184</v>
       </c>
-      <c r="B57" s="4" t="s">
+      <c r="B57" t="s">
         <v>197</v>
       </c>
-      <c r="C57" s="4" t="s">
+      <c r="C57" t="s">
         <v>214</v>
       </c>
-      <c r="E57" s="6" t="s">
+      <c r="D57" t="s">
+        <v>275</v>
+      </c>
+      <c r="E57" s="5" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="58" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A58" s="4" t="s">
+    <row r="58" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A58" t="s">
         <v>155</v>
       </c>
-      <c r="B58" s="4" t="s">
+      <c r="B58" t="s">
         <v>199</v>
       </c>
-      <c r="C58" s="4" t="s">
+      <c r="C58" t="s">
         <v>214</v>
       </c>
-      <c r="E58" s="6" t="s">
+      <c r="D58" t="s">
+        <v>276</v>
+      </c>
+      <c r="E58" s="5" t="s">
         <v>237</v>
       </c>
     </row>
-    <row r="59" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A59" s="4" t="s">
+    <row r="59" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A59" t="s">
         <v>185</v>
       </c>
-      <c r="B59" s="4" t="s">
+      <c r="B59" t="s">
         <v>200</v>
       </c>
-      <c r="C59" s="4" t="s">
+      <c r="C59" t="s">
         <v>214</v>
       </c>
-      <c r="E59" s="6" t="s">
+      <c r="D59" t="s">
+        <v>277</v>
+      </c>
+      <c r="E59" s="5" t="s">
         <v>238</v>
       </c>
     </row>
-    <row r="60" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A60" s="4" t="s">
+    <row r="60" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A60" t="s">
         <v>186</v>
       </c>
-      <c r="B60" s="4" t="s">
+      <c r="B60" t="s">
         <v>201</v>
       </c>
-      <c r="C60" s="4" t="s">
+      <c r="C60" t="s">
         <v>214</v>
       </c>
-      <c r="E60" s="6" t="s">
+      <c r="D60" t="s">
+        <v>278</v>
+      </c>
+      <c r="E60" s="5" t="s">
         <v>239</v>
       </c>
     </row>
-    <row r="61" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A61" s="4" t="s">
+    <row r="61" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A61" t="s">
         <v>187</v>
       </c>
-      <c r="B61" s="4" t="s">
+      <c r="B61" t="s">
         <v>198</v>
       </c>
-      <c r="C61" s="4" t="s">
+      <c r="C61" t="s">
         <v>214</v>
       </c>
-      <c r="E61" s="6" t="s">
+      <c r="D61" t="s">
+        <v>279</v>
+      </c>
+      <c r="E61" s="5" t="s">
         <v>240</v>
       </c>
     </row>
-    <row r="62" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A62" s="4" t="s">
+    <row r="62" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A62" t="s">
         <v>188</v>
       </c>
-      <c r="B62" s="4" t="s">
+      <c r="B62" t="s">
         <v>202</v>
       </c>
-      <c r="C62" s="4" t="s">
+      <c r="C62" t="s">
         <v>214</v>
       </c>
-      <c r="E62" s="6" t="s">
+      <c r="D62" t="s">
+        <v>280</v>
+      </c>
+      <c r="E62" s="5" t="s">
         <v>241</v>
       </c>
     </row>
-    <row r="63" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A63" s="4" t="s">
+    <row r="63" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A63" t="s">
         <v>147</v>
       </c>
-      <c r="B63" s="4" t="s">
+      <c r="B63" t="s">
         <v>203</v>
       </c>
-      <c r="C63" s="4" t="s">
+      <c r="C63" t="s">
         <v>214</v>
       </c>
-      <c r="E63" s="6" t="s">
+      <c r="D63" t="s">
+        <v>281</v>
+      </c>
+      <c r="E63" s="5" t="s">
         <v>242</v>
       </c>
     </row>
-    <row r="64" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A64" s="4" t="s">
+    <row r="64" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A64" t="s">
         <v>189</v>
       </c>
-      <c r="B64" s="4" t="s">
+      <c r="B64" t="s">
         <v>204</v>
       </c>
-      <c r="C64" s="4" t="s">
+      <c r="C64" t="s">
         <v>214</v>
       </c>
-      <c r="E64" s="6" t="s">
+      <c r="D64" t="s">
+        <v>282</v>
+      </c>
+      <c r="E64" s="5" t="s">
         <v>243</v>
       </c>
     </row>
-    <row r="65" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A65" s="4" t="s">
+    <row r="65" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A65" t="s">
         <v>190</v>
       </c>
-      <c r="B65" s="4" t="s">
+      <c r="B65" t="s">
         <v>205</v>
       </c>
-      <c r="C65" s="4" t="s">
+      <c r="C65" t="s">
         <v>214</v>
       </c>
-      <c r="E65" s="6" t="s">
+      <c r="D65" t="s">
+        <v>283</v>
+      </c>
+      <c r="E65" s="5" t="s">
         <v>244</v>
       </c>
     </row>
-    <row r="66" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A66" s="4" t="s">
+    <row r="66" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A66" t="s">
         <v>191</v>
       </c>
-      <c r="B66" s="4" t="s">
+      <c r="B66" t="s">
         <v>206</v>
       </c>
-      <c r="C66" s="4" t="s">
+      <c r="C66" t="s">
         <v>214</v>
       </c>
-      <c r="E66" s="6" t="s">
+      <c r="D66" t="s">
+        <v>284</v>
+      </c>
+      <c r="E66" s="5" t="s">
         <v>245</v>
       </c>
     </row>
-    <row r="67" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A67" s="4" t="s">
+    <row r="67" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A67" t="s">
         <v>192</v>
       </c>
-      <c r="B67" s="4" t="s">
+      <c r="B67" t="s">
         <v>207</v>
       </c>
-      <c r="C67" s="4" t="s">
+      <c r="C67" t="s">
         <v>214</v>
       </c>
-      <c r="E67" s="6" t="s">
+      <c r="D67" t="s">
+        <v>285</v>
+      </c>
+      <c r="E67" s="5" t="s">
         <v>246</v>
       </c>
     </row>
-    <row r="68" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A68" s="4" t="s">
+    <row r="68" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A68" t="s">
         <v>145</v>
       </c>
-      <c r="B68" s="4" t="s">
+      <c r="B68" t="s">
         <v>208</v>
       </c>
-      <c r="C68" s="4" t="s">
+      <c r="C68" t="s">
         <v>214</v>
       </c>
-      <c r="E68" s="6" t="s">
+      <c r="D68" t="s">
+        <v>286</v>
+      </c>
+      <c r="E68" s="5" t="s">
         <v>247</v>
       </c>
     </row>
-    <row r="69" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A69" s="4" t="s">
+    <row r="69" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A69" t="s">
         <v>193</v>
       </c>
-      <c r="B69" s="4" t="s">
+      <c r="B69" t="s">
         <v>209</v>
       </c>
-      <c r="C69" s="4" t="s">
+      <c r="C69" t="s">
         <v>214</v>
       </c>
-      <c r="E69" s="6" t="s">
+      <c r="D69" t="s">
+        <v>287</v>
+      </c>
+      <c r="E69" s="5" t="s">
         <v>248</v>
       </c>
     </row>
-    <row r="70" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A70" s="4" t="s">
+    <row r="70" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A70" t="s">
         <v>144</v>
       </c>
-      <c r="B70" s="4" t="s">
+      <c r="B70" t="s">
         <v>210</v>
       </c>
-      <c r="C70" s="4" t="s">
+      <c r="C70" t="s">
         <v>214</v>
       </c>
-      <c r="E70" s="6" t="s">
+      <c r="D70" t="s">
+        <v>288</v>
+      </c>
+      <c r="E70" s="5" t="s">
         <v>249</v>
       </c>
     </row>
-    <row r="71" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A71" s="4" t="s">
+    <row r="71" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A71" t="s">
         <v>194</v>
       </c>
-      <c r="B71" s="4" t="s">
+      <c r="B71" t="s">
         <v>211</v>
       </c>
-      <c r="C71" s="4" t="s">
+      <c r="C71" t="s">
         <v>214</v>
       </c>
-      <c r="E71" s="6" t="s">
+      <c r="D71" t="s">
+        <v>289</v>
+      </c>
+      <c r="E71" s="5" t="s">
         <v>250</v>
       </c>
     </row>
-    <row r="72" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A72" s="4" t="s">
+    <row r="72" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A72" t="s">
         <v>195</v>
       </c>
-      <c r="B72" s="4" t="s">
+      <c r="B72" t="s">
         <v>212</v>
       </c>
-      <c r="C72" s="4" t="s">
+      <c r="C72" t="s">
         <v>214</v>
       </c>
-      <c r="E72" s="6" t="s">
+      <c r="D72" t="s">
+        <v>290</v>
+      </c>
+      <c r="E72" s="5" t="s">
         <v>251</v>
       </c>
     </row>
-    <row r="73" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A73" s="4" t="s">
+    <row r="73" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A73" t="s">
         <v>196</v>
       </c>
-      <c r="B73" s="4" t="s">
+      <c r="B73" t="s">
         <v>213</v>
       </c>
-      <c r="C73" s="4" t="s">
+      <c r="C73" t="s">
         <v>214</v>
       </c>
-      <c r="E73" s="6" t="s">
+      <c r="D73" t="s">
+        <v>291</v>
+      </c>
+      <c r="E73" s="5" t="s">
         <v>252</v>
       </c>
     </row>
-    <row r="74" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="75" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="76" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="77" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="78" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="79" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="80" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="81" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="82" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="83" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="84" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="85" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="86" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="87" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="88" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="89" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="90" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="91" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="92" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="93" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="94" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="95" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="96" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="97" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="98" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="99" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="100" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="101" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="102" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="103" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="104" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="105" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="106" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="107" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="108" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="109" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="110" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="111" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="112" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="113" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="114" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="115" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="116" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="117" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="118" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="119" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="120" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="121" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="122" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="123" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="124" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="125" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="126" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="127" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="128" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="129" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="130" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="131" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="132" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="133" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="134" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="135" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="136" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="137" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="138" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="139" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="140" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="141" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="142" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="143" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="144" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="145" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="146" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="147" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="148" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="149" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="150" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="151" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="152" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="153" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="154" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="155" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="156" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="157" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="158" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="159" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="160" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="161" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="162" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="163" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="164" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="165" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="166" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="167" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="168" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="169" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="170" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="171" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="172" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="173" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="174" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="175" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="176" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="177" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="178" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="179" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="180" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="181" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="182" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="183" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="184" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="185" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="186" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="187" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="188" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="189" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="190" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="191" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="192" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="193" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="194" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="195" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="196" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="197" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="198" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="199" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="200" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="201" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="202" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="203" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="204" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="205" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="206" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="207" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="208" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="209" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="210" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="211" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="212" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="213" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="214" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="215" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="216" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="217" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="218" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="219" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="220" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="221" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="222" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="223" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="224" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="225" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="226" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="227" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="228" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="229" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="230" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="231" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="232" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="233" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="234" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="235" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="236" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="237" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="238" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="239" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="240" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="241" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="242" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="243" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="244" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="245" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="246" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="247" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="248" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="249" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="250" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="251" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="252" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="253" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="254" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="255" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="256" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="257" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="258" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="259" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="260" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="261" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="262" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="263" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="264" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="265" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="266" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="267" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="268" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="269" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="270" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="271" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="272" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="273" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="274" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="275" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="276" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="277" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="278" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="279" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="280" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="281" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="282" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="283" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="284" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="285" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="286" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="287" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="288" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="289" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="290" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="291" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="292" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="293" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="294" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="295" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="296" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="297" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="298" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="299" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="300" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="301" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="302" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="303" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="304" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="305" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="306" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="307" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="308" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="309" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="310" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="311" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="312" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="313" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="314" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="315" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="316" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="317" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="318" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="319" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="320" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="321" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="322" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="323" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="324" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="325" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="326" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="327" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="328" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="329" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="330" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="331" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="332" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="333" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="334" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="335" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="336" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="337" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="338" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="339" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="340" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="341" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="342" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="343" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="344" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="345" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="346" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="347" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="348" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="349" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="350" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="351" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="352" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="353" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="354" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="355" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="356" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="357" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="358" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="359" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="360" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="361" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="362" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="363" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="364" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="365" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="366" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="367" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="368" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="369" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="370" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="371" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="372" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="373" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="374" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="375" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="376" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="377" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="378" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="379" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="380" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="381" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="382" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="383" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="384" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="385" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="386" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="387" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="388" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="389" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="390" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="391" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="392" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="393" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="394" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="395" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="396" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="397" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="398" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="399" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="400" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="401" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="402" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="403" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="404" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="405" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="406" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="407" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="408" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="409" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="410" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="411" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="412" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="413" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="414" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="415" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="416" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="417" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="418" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="419" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="420" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="421" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="422" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="423" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="424" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="425" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="426" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="427" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="428" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="429" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="430" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="431" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="432" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="433" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="434" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="435" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="436" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="437" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="438" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="439" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="440" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="441" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="442" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="443" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="444" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="445" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="446" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="447" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="448" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="449" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="450" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="451" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="452" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="453" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="454" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="455" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="456" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="457" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="458" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="459" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="460" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="461" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="462" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="463" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="464" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="465" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="466" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="467" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="468" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="469" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="470" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="471" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="472" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="473" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="474" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="475" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="476" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="477" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="478" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="479" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="480" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="481" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="482" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="483" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="484" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="485" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="486" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="487" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="488" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="489" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="490" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="491" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="492" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="493" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="494" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="495" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="496" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="497" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="498" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="499" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="500" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="501" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="502" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="503" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="504" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="505" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="506" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="507" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="508" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="509" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="510" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="511" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="512" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="513" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="514" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="515" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="516" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="517" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="518" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="519" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="520" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="521" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="522" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="523" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="524" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="525" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="526" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="527" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="528" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="529" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="530" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="531" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="532" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="533" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="534" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="535" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="536" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="537" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="538" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="539" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="540" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="541" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="542" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="543" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="544" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="545" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="546" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="547" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="548" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="549" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="550" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="551" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="552" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="553" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="554" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="555" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="556" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="557" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="558" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="559" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="560" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="561" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="562" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="563" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="564" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="565" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="566" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="567" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="568" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="569" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="570" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="571" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="572" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="573" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="574" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="575" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="576" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="577" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="578" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="579" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="580" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="581" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="582" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="583" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="584" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="585" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="586" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="587" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="588" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="589" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="590" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="591" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="592" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="593" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="594" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="595" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="596" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="597" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="598" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="599" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="600" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="601" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="602" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="603" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="604" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="605" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="606" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="607" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="608" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="609" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="610" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="611" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="612" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="613" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="614" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="615" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="616" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="617" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="618" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="619" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="620" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="621" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="622" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="623" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="624" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="625" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="626" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="627" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="628" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="629" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="630" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="631" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="632" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="633" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="634" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="635" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="636" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="637" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="638" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="639" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="640" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="641" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="642" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="643" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="644" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="645" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="646" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="647" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="648" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="649" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="650" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="651" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="652" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="653" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="654" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="655" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="656" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="657" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="658" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="659" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="660" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="661" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="662" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="663" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="664" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="665" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="666" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="667" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="668" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="669" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="670" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="671" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="672" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="673" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="674" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="675" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="676" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="677" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="678" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="679" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="680" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="681" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="682" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="683" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="684" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="685" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="686" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="687" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="688" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="689" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="690" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="691" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="692" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="693" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="694" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="695" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="696" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="697" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="698" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="699" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="700" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="701" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="702" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="703" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="704" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="705" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="706" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="707" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="708" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="709" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="710" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="711" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="712" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="713" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="714" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="715" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="716" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="717" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="718" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="719" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="720" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="721" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="722" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="723" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="724" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="725" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="726" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="727" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="728" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="729" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="730" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="731" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="732" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="733" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="734" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="735" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="736" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="737" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="738" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="739" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="740" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="741" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="742" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="743" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="744" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="745" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="746" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="747" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="748" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="749" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="750" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="751" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="752" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="753" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="754" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="755" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="756" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="757" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="758" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="759" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="760" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="761" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="762" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="763" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="764" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="765" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="766" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="767" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="768" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="769" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="770" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="771" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="772" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="773" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="774" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="775" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="776" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="777" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="778" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="779" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="780" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="781" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="782" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="783" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="784" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="785" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="786" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="787" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="788" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="789" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="790" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="791" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="792" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="793" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="794" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="795" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="796" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="797" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="798" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="799" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="800" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="801" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="802" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="803" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="804" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="805" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="806" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="807" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="808" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="809" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="810" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="811" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="812" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="813" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="814" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="815" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="816" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="817" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="818" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="819" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="820" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="821" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="822" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="823" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="824" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="825" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="826" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="827" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="828" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="829" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="830" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="831" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="832" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="833" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="834" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="835" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="836" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="837" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="838" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="839" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="840" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="841" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="842" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="843" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="844" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="845" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="846" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="847" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="848" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="849" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="850" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="851" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="852" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="853" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="854" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="855" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="856" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="857" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="858" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="859" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="860" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="861" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="862" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="863" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="864" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="865" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="866" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="867" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="868" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="869" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="870" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="871" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="872" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="873" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="874" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="875" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="876" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="877" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="878" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="879" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="880" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="881" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="882" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="883" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="884" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="885" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="886" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="887" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="888" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="889" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="890" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="891" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="892" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="893" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="894" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="895" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="896" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="897" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="898" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="899" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="900" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="901" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="902" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="903" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="904" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="905" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="906" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="907" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="908" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="909" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="910" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="911" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="912" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="913" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="914" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="915" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="916" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="917" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="918" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="919" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="920" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="921" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="922" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="923" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="924" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="925" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="926" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="927" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="928" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="929" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="930" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="931" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="932" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="933" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="934" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="935" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="936" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="937" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="938" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="939" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="940" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="941" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="942" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="943" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="944" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="945" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="946" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="947" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="948" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="949" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="950" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="951" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="952" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="953" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="954" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="955" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="956" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="957" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="958" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="959" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="960" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="961" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="962" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="963" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="964" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="965" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="966" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="967" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="968" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="969" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="970" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="971" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="972" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="973" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="974" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="975" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="976" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="977" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="978" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="979" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="980" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="981" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="982" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="983" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="984" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="985" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="986" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="987" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="988" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="989" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="990" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="991" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="992" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="993" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="994" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="995" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="996" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="997" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="998" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="999" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="1000" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="74" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="75" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="76" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="77" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="78" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="79" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="80" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="81" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="82" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="83" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="84" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="85" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="86" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="87" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="88" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="89" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="90" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="91" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="92" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="93" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="94" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="95" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="96" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="97" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="98" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="99" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="100" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="101" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="102" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="103" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="104" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="105" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="106" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="107" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="108" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="109" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="110" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="111" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="112" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="113" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="114" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="115" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="116" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="117" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="118" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="119" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="120" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="121" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="122" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="123" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="124" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="125" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="126" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="127" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="128" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="129" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="130" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="131" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="132" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="133" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="134" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="135" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="136" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="137" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="138" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="139" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="140" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="141" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="142" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="143" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="144" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="145" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="146" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="147" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="148" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="149" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="150" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="151" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="152" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="153" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="154" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="155" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="156" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="157" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="158" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="159" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="160" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="161" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="162" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="163" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="164" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="165" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="166" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="167" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="168" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="169" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="170" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="171" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="172" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="173" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="174" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="175" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="176" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="177" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="178" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="179" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="180" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="181" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="182" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="183" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="184" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="185" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="186" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="187" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="188" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="189" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="190" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="191" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="192" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="193" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="194" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="195" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="196" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="197" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="198" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="199" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="200" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="201" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="202" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="203" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="204" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="205" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="206" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="207" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="208" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="209" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="210" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="211" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="212" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="213" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="214" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="215" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="216" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="217" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="218" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="219" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="220" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="221" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="222" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="223" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="224" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="225" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="226" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="227" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="228" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="229" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="230" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="231" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="232" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="233" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="234" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="235" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="236" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="237" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="238" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="239" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="240" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="241" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="242" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="243" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="244" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="245" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="246" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="247" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="248" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="249" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="250" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="251" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="252" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="253" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="254" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="255" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="256" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="257" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="258" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="259" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="260" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="261" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="262" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="263" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="264" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="265" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="266" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="267" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="268" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="269" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="270" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="271" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="272" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="273" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="274" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="275" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="276" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="277" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="278" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="279" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="280" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="281" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="282" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="283" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="284" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="285" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="286" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="287" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="288" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="289" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="290" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="291" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="292" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="293" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="294" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="295" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="296" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="297" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="298" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="299" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="300" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="301" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="302" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="303" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="304" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="305" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="306" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="307" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="308" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="309" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="310" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="311" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="312" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="313" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="314" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="315" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="316" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="317" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="318" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="319" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="320" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="321" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="322" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="323" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="324" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="325" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="326" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="327" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="328" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="329" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="330" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="331" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="332" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="333" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="334" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="335" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="336" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="337" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="338" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="339" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="340" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="341" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="342" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="343" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="344" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="345" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="346" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="347" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="348" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="349" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="350" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="351" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="352" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="353" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="354" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="355" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="356" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="357" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="358" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="359" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="360" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="361" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="362" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="363" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="364" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="365" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="366" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="367" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="368" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="369" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="370" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="371" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="372" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="373" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="374" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="375" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="376" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="377" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="378" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="379" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="380" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="381" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="382" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="383" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="384" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="385" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="386" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="387" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="388" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="389" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="390" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="391" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="392" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="393" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="394" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="395" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="396" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="397" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="398" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="399" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="400" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="401" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="402" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="403" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="404" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="405" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="406" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="407" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="408" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="409" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="410" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="411" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="412" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="413" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="414" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="415" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="416" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="417" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="418" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="419" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="420" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="421" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="422" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="423" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="424" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="425" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="426" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="427" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="428" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="429" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="430" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="431" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="432" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="433" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="434" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="435" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="436" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="437" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="438" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="439" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="440" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="441" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="442" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="443" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="444" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="445" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="446" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="447" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="448" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="449" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="450" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="451" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="452" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="453" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="454" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="455" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="456" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="457" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="458" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="459" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="460" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="461" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="462" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="463" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="464" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="465" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="466" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="467" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="468" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="469" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="470" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="471" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="472" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="473" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="474" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="475" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="476" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="477" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="478" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="479" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="480" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="481" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="482" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="483" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="484" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="485" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="486" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="487" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="488" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="489" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="490" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="491" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="492" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="493" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="494" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="495" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="496" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="497" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="498" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="499" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="500" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="501" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="502" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="503" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="504" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="505" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="506" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="507" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="508" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="509" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="510" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="511" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="512" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="513" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="514" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="515" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="516" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="517" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="518" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="519" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="520" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="521" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="522" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="523" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="524" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="525" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="526" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="527" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="528" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="529" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="530" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="531" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="532" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="533" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="534" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="535" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="536" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="537" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="538" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="539" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="540" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="541" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="542" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="543" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="544" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="545" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="546" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="547" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="548" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="549" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="550" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="551" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="552" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="553" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="554" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="555" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="556" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="557" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="558" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="559" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="560" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="561" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="562" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="563" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="564" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="565" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="566" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="567" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="568" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="569" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="570" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="571" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="572" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="573" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="574" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="575" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="576" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="577" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="578" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="579" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="580" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="581" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="582" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="583" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="584" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="585" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="586" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="587" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="588" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="589" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="590" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="591" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="592" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="593" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="594" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="595" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="596" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="597" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="598" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="599" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="600" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="601" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="602" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="603" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="604" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="605" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="606" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="607" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="608" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="609" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="610" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="611" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="612" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="613" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="614" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="615" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="616" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="617" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="618" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="619" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="620" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="621" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="622" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="623" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="624" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="625" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="626" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="627" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="628" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="629" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="630" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="631" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="632" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="633" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="634" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="635" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="636" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="637" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="638" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="639" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="640" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="641" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="642" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="643" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="644" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="645" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="646" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="647" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="648" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="649" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="650" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="651" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="652" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="653" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="654" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="655" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="656" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="657" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="658" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="659" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="660" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="661" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="662" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="663" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="664" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="665" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="666" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="667" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="668" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="669" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="670" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="671" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="672" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="673" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="674" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="675" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="676" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="677" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="678" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="679" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="680" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="681" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="682" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="683" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="684" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="685" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="686" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="687" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="688" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="689" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="690" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="691" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="692" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="693" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="694" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="695" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="696" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="697" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="698" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="699" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="700" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="701" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="702" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="703" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="704" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="705" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="706" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="707" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="708" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="709" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="710" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="711" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="712" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="713" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="714" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="715" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="716" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="717" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="718" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="719" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="720" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="721" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="722" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="723" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="724" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="725" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="726" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="727" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="728" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="729" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="730" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="731" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="732" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="733" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="734" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="735" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="736" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="737" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="738" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="739" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="740" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="741" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="742" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="743" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="744" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="745" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="746" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="747" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="748" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="749" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="750" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="751" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="752" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="753" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="754" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="755" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="756" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="757" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="758" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="759" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="760" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="761" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="762" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="763" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="764" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="765" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="766" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="767" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="768" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="769" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="770" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="771" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="772" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="773" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="774" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="775" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="776" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="777" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="778" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="779" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="780" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="781" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="782" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="783" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="784" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="785" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="786" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="787" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="788" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="789" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="790" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="791" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="792" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="793" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="794" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="795" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="796" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="797" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="798" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="799" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="800" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="801" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="802" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="803" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="804" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="805" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="806" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="807" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="808" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="809" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="810" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="811" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="812" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="813" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="814" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="815" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="816" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="817" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="818" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="819" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="820" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="821" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="822" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="823" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="824" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="825" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="826" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="827" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="828" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="829" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="830" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="831" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="832" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="833" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="834" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="835" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="836" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="837" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="838" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="839" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="840" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="841" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="842" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="843" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="844" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="845" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="846" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="847" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="848" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="849" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="850" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="851" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="852" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="853" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="854" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="855" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="856" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="857" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="858" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="859" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="860" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="861" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="862" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="863" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="864" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="865" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="866" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="867" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="868" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="869" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="870" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="871" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="872" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="873" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="874" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="875" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="876" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="877" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="878" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="879" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="880" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="881" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="882" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="883" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="884" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="885" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="886" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="887" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="888" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="889" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="890" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="891" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="892" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="893" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="894" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="895" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="896" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="897" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="898" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="899" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="900" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="901" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="902" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="903" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="904" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="905" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="906" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="907" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="908" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="909" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="910" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="911" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="912" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="913" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="914" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="915" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="916" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="917" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="918" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="919" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="920" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="921" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="922" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="923" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="924" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="925" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="926" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="927" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="928" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="929" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="930" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="931" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="932" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="933" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="934" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="935" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="936" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="937" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="938" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="939" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="940" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="941" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="942" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="943" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="944" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="945" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="946" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="947" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="948" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="949" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="950" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="951" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="952" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="953" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="954" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="955" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="956" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="957" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="958" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="959" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="960" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="961" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="962" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="963" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="964" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="965" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="966" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="967" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="968" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="969" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="970" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="971" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="972" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="973" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="974" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="975" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="976" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="977" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="978" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="979" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="980" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="981" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="982" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="983" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="984" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="985" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="986" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="987" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="988" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="989" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="990" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="991" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="992" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="993" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="994" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="995" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="996" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="997" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="998" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="999" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="1000" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="D5" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>

</xml_diff>

<commit_message>
Preparing to add images for Numbers
</commit_message>
<xml_diff>
--- a/hmoob_lus/PDF HLLA.xlsx
+++ b/hmoob_lus/PDF HLLA.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ntxhw\Desktop\Projects\HLLA\hmoob_lus\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D91DE358-E6B8-4E03-827D-7C82CDAA6775}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6397D342-0863-4FE5-A401-9BAA20B909B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-90" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="361" uniqueCount="291">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="372" uniqueCount="302">
   <si>
     <t>English Word</t>
   </si>
@@ -898,6 +898,39 @@
   </si>
   <si>
     <t>Image Filename</t>
+  </si>
+  <si>
+    <t>0.png</t>
+  </si>
+  <si>
+    <t>1.png</t>
+  </si>
+  <si>
+    <t>2.png</t>
+  </si>
+  <si>
+    <t>3.png</t>
+  </si>
+  <si>
+    <t>4.png</t>
+  </si>
+  <si>
+    <t>5.png</t>
+  </si>
+  <si>
+    <t>6.png</t>
+  </si>
+  <si>
+    <t>7.png</t>
+  </si>
+  <si>
+    <t>8.png</t>
+  </si>
+  <si>
+    <t>9.png</t>
+  </si>
+  <si>
+    <t>10.png</t>
   </si>
 </sst>
 </file>
@@ -1208,7 +1241,7 @@
   <dimension ref="A1:J1000"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="63" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="M6" sqref="M6"/>
+      <selection activeCell="I18" sqref="I18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1357,6 +1390,9 @@
       <c r="E7" s="2" t="s">
         <v>33</v>
       </c>
+      <c r="I7" t="s">
+        <v>291</v>
+      </c>
     </row>
     <row r="8" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
@@ -1374,6 +1410,9 @@
       <c r="E8" s="2" t="s">
         <v>37</v>
       </c>
+      <c r="I8" t="s">
+        <v>292</v>
+      </c>
     </row>
     <row r="9" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
@@ -1391,6 +1430,9 @@
       <c r="E9" s="2" t="s">
         <v>41</v>
       </c>
+      <c r="I9" t="s">
+        <v>293</v>
+      </c>
     </row>
     <row r="10" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
@@ -1408,6 +1450,9 @@
       <c r="E10" s="2" t="s">
         <v>45</v>
       </c>
+      <c r="I10" t="s">
+        <v>294</v>
+      </c>
     </row>
     <row r="11" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
@@ -1425,6 +1470,9 @@
       <c r="E11" s="2" t="s">
         <v>49</v>
       </c>
+      <c r="I11" t="s">
+        <v>295</v>
+      </c>
     </row>
     <row r="12" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
@@ -1442,6 +1490,9 @@
       <c r="E12" s="2" t="s">
         <v>53</v>
       </c>
+      <c r="I12" t="s">
+        <v>296</v>
+      </c>
     </row>
     <row r="13" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
@@ -1459,6 +1510,9 @@
       <c r="E13" s="2" t="s">
         <v>57</v>
       </c>
+      <c r="I13" t="s">
+        <v>297</v>
+      </c>
     </row>
     <row r="14" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
@@ -1476,6 +1530,9 @@
       <c r="E14" s="2" t="s">
         <v>61</v>
       </c>
+      <c r="I14" t="s">
+        <v>298</v>
+      </c>
     </row>
     <row r="15" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
@@ -1493,6 +1550,9 @@
       <c r="E15" s="2" t="s">
         <v>65</v>
       </c>
+      <c r="I15" t="s">
+        <v>299</v>
+      </c>
     </row>
     <row r="16" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
@@ -1510,8 +1570,11 @@
       <c r="E16" s="2" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="17" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I16" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>70</v>
       </c>
@@ -1527,8 +1590,11 @@
       <c r="E17" s="2" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="18" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I17" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>74</v>
       </c>
@@ -1545,7 +1611,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="19" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>79</v>
       </c>
@@ -1562,7 +1628,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="20" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>83</v>
       </c>
@@ -1579,7 +1645,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="21" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>87</v>
       </c>
@@ -1596,7 +1662,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="22" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>91</v>
       </c>
@@ -1613,7 +1679,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="23" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
         <v>96</v>
       </c>
@@ -1630,7 +1696,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="24" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
         <v>100</v>
       </c>
@@ -1644,7 +1710,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="25" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
         <v>103</v>
       </c>
@@ -1658,7 +1724,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="26" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
         <v>106</v>
       </c>
@@ -1672,7 +1738,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="27" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
         <v>109</v>
       </c>
@@ -1686,7 +1752,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="28" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
         <v>112</v>
       </c>
@@ -1700,7 +1766,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="29" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
         <v>115</v>
       </c>
@@ -1714,7 +1780,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="30" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
         <v>118</v>
       </c>
@@ -1728,7 +1794,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="31" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
         <v>121</v>
       </c>
@@ -1742,7 +1808,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="32" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
         <v>124</v>
       </c>

</xml_diff>

<commit_message>
Change consonant to single consonant in pdf
</commit_message>
<xml_diff>
--- a/hmoob_lus/PDF HLLA.xlsx
+++ b/hmoob_lus/PDF HLLA.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ntxhw\Desktop\Projects\HLLA\hmoob_lus\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{908FC255-8B7D-4DB4-8967-82750763F234}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E87FCBFE-8B23-4CE2-95A5-79C7417E8168}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -361,6 +361,9 @@
     <t>Female - Mom.wav</t>
   </si>
   <si>
+    <t>mother.png</t>
+  </si>
+  <si>
     <t>father</t>
   </si>
   <si>
@@ -373,6 +376,9 @@
     <t>Female - Dad.wav</t>
   </si>
   <si>
+    <t>father.png</t>
+  </si>
+  <si>
     <t>older brother (female use)</t>
   </si>
   <si>
@@ -382,6 +388,9 @@
     <t>Female - Older Brother.wav</t>
   </si>
   <si>
+    <t>older brother.png</t>
+  </si>
+  <si>
     <t>younger brother (female use)</t>
   </si>
   <si>
@@ -391,6 +400,9 @@
     <t>Female - Younger Brother.wav</t>
   </si>
   <si>
+    <t>younger brother.png</t>
+  </si>
+  <si>
     <t>older sister (female use)</t>
   </si>
   <si>
@@ -400,6 +412,9 @@
     <t>Female - Older Sister.wav</t>
   </si>
   <si>
+    <t>older sister.png</t>
+  </si>
+  <si>
     <t>younger sister (female use)</t>
   </si>
   <si>
@@ -409,6 +424,9 @@
     <t>Female - Younger Sister.wav</t>
   </si>
   <si>
+    <t>younger sister.png</t>
+  </si>
+  <si>
     <t>older brother (male use)</t>
   </si>
   <si>
@@ -457,6 +475,9 @@
     <t>Female - Maternal Auntie or Grandmother.wav</t>
   </si>
   <si>
+    <t>maternal grandmother.png</t>
+  </si>
+  <si>
     <t>grandfather (maternal)</t>
   </si>
   <si>
@@ -469,6 +490,9 @@
     <t>Female - Maternal Grandfather.wav</t>
   </si>
   <si>
+    <t>maternal grandfather.png</t>
+  </si>
+  <si>
     <t>grandmother (paternal)</t>
   </si>
   <si>
@@ -481,6 +505,9 @@
     <t>Female - Paternal Grandmother.wav</t>
   </si>
   <si>
+    <t>paternal grandmother.png</t>
+  </si>
+  <si>
     <t>grandfather (paternal)</t>
   </si>
   <si>
@@ -493,6 +520,9 @@
     <t>Female - Paternal Grandfather.wav</t>
   </si>
   <si>
+    <t>paternal grandfather.png</t>
+  </si>
+  <si>
     <t>b</t>
   </si>
   <si>
@@ -502,48 +532,96 @@
     <t>Tone Markers</t>
   </si>
   <si>
+    <t>Male - Tone Marker B.wav</t>
+  </si>
+  <si>
+    <t>Female - Tone Marker B.wav</t>
+  </si>
+  <si>
     <t>j</t>
   </si>
   <si>
     <t>cim ntuj</t>
   </si>
   <si>
+    <t>Male - Tone Marker J.wav</t>
+  </si>
+  <si>
+    <t>Female - Tone Marker J.wav</t>
+  </si>
+  <si>
     <t>v</t>
   </si>
   <si>
     <t>cim kuv</t>
   </si>
   <si>
+    <t>Male - Tone Marker V.wav</t>
+  </si>
+  <si>
+    <t>Female - Tone Marker V.wav</t>
+  </si>
+  <si>
     <t>s</t>
   </si>
   <si>
     <t>cim mus</t>
   </si>
   <si>
+    <t>Male - Tone Marker S.wav</t>
+  </si>
+  <si>
+    <t>Female - Tone Marker S.wav</t>
+  </si>
+  <si>
     <t>g</t>
   </si>
   <si>
     <t>cim neeg</t>
   </si>
   <si>
+    <t>Male - Tone Marker G.wav</t>
+  </si>
+  <si>
+    <t>Female - Tone Marker G.wav</t>
+  </si>
+  <si>
     <t>m</t>
   </si>
   <si>
     <t>cim niam</t>
   </si>
   <si>
+    <t>Male - Tone Marker M.wav</t>
+  </si>
+  <si>
+    <t>Female - Tone Marker M.wav</t>
+  </si>
+  <si>
     <t>d</t>
   </si>
   <si>
     <t>cim tod</t>
   </si>
   <si>
+    <t>Male - Tone Marker D.wav</t>
+  </si>
+  <si>
+    <t>Female - Tone Marker D.wav</t>
+  </si>
+  <si>
     <t>(-)/no tone</t>
   </si>
   <si>
     <t>cim ua</t>
   </si>
   <si>
+    <t>Male - Tone Marker (-).wav</t>
+  </si>
+  <si>
+    <t>Female - Tone Marker (-).wav</t>
+  </si>
+  <si>
     <t>a</t>
   </si>
   <si>
@@ -553,75 +631,153 @@
     <t>Single Vowels</t>
   </si>
   <si>
+    <t>Male - Single Vowel A.wav</t>
+  </si>
+  <si>
+    <t>Female - Single Vowel A.wav</t>
+  </si>
+  <si>
     <t>e</t>
   </si>
   <si>
     <t>say</t>
   </si>
   <si>
+    <t>Male - Single Vowel E.wav</t>
+  </si>
+  <si>
+    <t>Female - Single Vowel E.wav</t>
+  </si>
+  <si>
     <t>i</t>
   </si>
   <si>
     <t>tea</t>
   </si>
   <si>
+    <t>Male - Single Vowel I.wav</t>
+  </si>
+  <si>
+    <t>Female - Single Vowel I.wav</t>
+  </si>
+  <si>
     <t>o</t>
   </si>
   <si>
+    <t>Male - Single Vowel O.wav</t>
+  </si>
+  <si>
+    <t>Female - Single Vowel O.wav</t>
+  </si>
+  <si>
     <t>u</t>
   </si>
   <si>
     <t>you</t>
   </si>
   <si>
+    <t>Male - Single Vowel U.wav</t>
+  </si>
+  <si>
+    <t>Female - Single Vowel U.wav</t>
+  </si>
+  <si>
     <t>w</t>
   </si>
   <si>
     <t>could</t>
   </si>
   <si>
+    <t>Male - Single Vowel W.wav</t>
+  </si>
+  <si>
+    <t>Female - Single Vowel W.wav</t>
+  </si>
+  <si>
     <t>ai</t>
   </si>
   <si>
     <t>Double Vowels</t>
   </si>
   <si>
+    <t>Male - Double Vowel AI.wav</t>
+  </si>
+  <si>
+    <t>Female - Double Vowel AI.wav</t>
+  </si>
+  <si>
     <t>au</t>
   </si>
   <si>
     <t>tau</t>
   </si>
   <si>
+    <t>Male - Double Vowel AU.wav</t>
+  </si>
+  <si>
+    <t>Female - Double  Vowel AU.wav</t>
+  </si>
+  <si>
     <t>aw</t>
   </si>
   <si>
     <t>taw</t>
   </si>
   <si>
+    <t>Male - Double Vowel AW.wav</t>
+  </si>
+  <si>
+    <t>Female - Double  Vowel AW.wav</t>
+  </si>
+  <si>
     <t>ee</t>
   </si>
   <si>
     <t>yeej</t>
   </si>
   <si>
+    <t>Male - Double Vowel EE.wav</t>
+  </si>
+  <si>
+    <t>Female - Double  Vowel EE.wav</t>
+  </si>
+  <si>
     <t>ia</t>
   </si>
   <si>
     <t>dhia</t>
   </si>
   <si>
+    <t>Male - Double Vowel IA.wav</t>
+  </si>
+  <si>
+    <t>Female - Double  Vowel IA.wav</t>
+  </si>
+  <si>
     <t>oo</t>
   </si>
   <si>
     <t>zoo</t>
   </si>
   <si>
+    <t>Male - Double Vowel OO.wav</t>
+  </si>
+  <si>
+    <t>Female - Double  Vowel OO.wav</t>
+  </si>
+  <si>
     <t>ua</t>
   </si>
   <si>
     <t>cua</t>
   </si>
   <si>
+    <t>Male - Double Vowel UA.wav</t>
+  </si>
+  <si>
+    <t>Female - Double  Vowel UA.wav</t>
+  </si>
+  <si>
     <t>c</t>
   </si>
   <si>
@@ -634,6 +790,9 @@
     <t>dos dev</t>
   </si>
   <si>
+    <t>Female - Consonant D.wav</t>
+  </si>
+  <si>
     <t>f</t>
   </si>
   <si>
@@ -646,6 +805,9 @@
     <t>hos haus</t>
   </si>
   <si>
+    <t>Female - Consonant H.wav</t>
+  </si>
+  <si>
     <t>k</t>
   </si>
   <si>
@@ -658,6 +820,9 @@
     <t>los liab</t>
   </si>
   <si>
+    <t>Female - Consonant L.wav</t>
+  </si>
+  <si>
     <t>mos miv</t>
   </si>
   <si>
@@ -667,6 +832,9 @@
     <t>nos noog</t>
   </si>
   <si>
+    <t>Female - Consonant N.wav</t>
+  </si>
+  <si>
     <t>p</t>
   </si>
   <si>
@@ -679,6 +847,9 @@
     <t xml:space="preserve">qos qav </t>
   </si>
   <si>
+    <t>Female - Consonant Q.wav</t>
+  </si>
+  <si>
     <t>r</t>
   </si>
   <si>
@@ -694,6 +865,9 @@
     <t>tos twm</t>
   </si>
   <si>
+    <t>Female - Consonant T.wav</t>
+  </si>
+  <si>
     <t>vos vas</t>
   </si>
   <si>
@@ -715,269 +889,95 @@
     <t>zos zeb</t>
   </si>
   <si>
-    <t>mother.png</t>
-  </si>
-  <si>
-    <t>father.png</t>
-  </si>
-  <si>
-    <t>older brother.png</t>
-  </si>
-  <si>
-    <t>younger brother.png</t>
-  </si>
-  <si>
-    <t>older sister.png</t>
-  </si>
-  <si>
-    <t>younger sister.png</t>
-  </si>
-  <si>
-    <t>maternal grandmother.png</t>
-  </si>
-  <si>
-    <t>maternal grandfather.png</t>
-  </si>
-  <si>
-    <t>paternal grandmother.png</t>
-  </si>
-  <si>
-    <t>paternal grandfather.png</t>
-  </si>
-  <si>
-    <t>Female - Double Vowel AI.wav</t>
-  </si>
-  <si>
-    <t>Female - Tone Marker B.wav</t>
-  </si>
-  <si>
-    <t>Female - Tone Marker J.wav</t>
-  </si>
-  <si>
-    <t>Female - Tone Marker V.wav</t>
-  </si>
-  <si>
-    <t>Female - Consonant Z.wav</t>
-  </si>
-  <si>
-    <t>Female - Consonant Y.wav</t>
-  </si>
-  <si>
-    <t>Female - Consonant X.wav</t>
-  </si>
-  <si>
-    <t>Female - Consonant V.wav</t>
-  </si>
-  <si>
-    <t>Female - Consonant T.wav</t>
-  </si>
-  <si>
-    <t>Female - Consonant S.wav</t>
-  </si>
-  <si>
-    <t>Female - Consonant R.wav</t>
-  </si>
-  <si>
-    <t>Female - Tone Marker G.wav</t>
-  </si>
-  <si>
-    <t>Female - Tone Marker S.wav</t>
-  </si>
-  <si>
-    <t>Female - Tone Marker M.wav</t>
-  </si>
-  <si>
-    <t>Female - Tone Marker D.wav</t>
-  </si>
-  <si>
-    <t>Female - Tone Marker (-).wav</t>
-  </si>
-  <si>
-    <t>Female - Single Vowel A.wav</t>
-  </si>
-  <si>
-    <t>Female - Single Vowel E.wav</t>
-  </si>
-  <si>
-    <t>Female - Single Vowel I.wav</t>
-  </si>
-  <si>
-    <t>Female - Single Vowel O.wav</t>
-  </si>
-  <si>
-    <t>Female - Single Vowel U.wav</t>
-  </si>
-  <si>
-    <t>Female - Single Vowel W.wav</t>
-  </si>
-  <si>
-    <t>Female - Double  Vowel AW.wav</t>
-  </si>
-  <si>
-    <t>Female - Double  Vowel EE.wav</t>
-  </si>
-  <si>
-    <t>Female - Double  Vowel AU.wav</t>
-  </si>
-  <si>
-    <t>Female - Double  Vowel IA.wav</t>
-  </si>
-  <si>
-    <t>Female - Double  Vowel OO.wav</t>
-  </si>
-  <si>
-    <t>Female - Double  Vowel UA.wav</t>
-  </si>
-  <si>
-    <t>Female - Consonant C.wav</t>
-  </si>
-  <si>
-    <t>Female - Consonant D.wav</t>
-  </si>
-  <si>
-    <t>Female - Consonant F.wav</t>
-  </si>
-  <si>
-    <t>Female - Consonant H.wav</t>
-  </si>
-  <si>
-    <t>Female - Consonant K.wav</t>
-  </si>
-  <si>
-    <t>Female - Consonant L.wav</t>
-  </si>
-  <si>
-    <t>Female - Consonant M.wav</t>
-  </si>
-  <si>
-    <t>Female - Consonant N.wav</t>
-  </si>
-  <si>
-    <t>Female - Consonant P.wav</t>
-  </si>
-  <si>
-    <t>Female - Consonant Q.wav</t>
-  </si>
-  <si>
-    <t>Male - Tone Marker B.wav</t>
-  </si>
-  <si>
-    <t>Male - Tone Marker J.wav</t>
-  </si>
-  <si>
-    <t>Male - Tone Marker V.wav</t>
-  </si>
-  <si>
-    <t>Male - Tone Marker S.wav</t>
-  </si>
-  <si>
-    <t>Male - Tone Marker G.wav</t>
-  </si>
-  <si>
-    <t>Male - Tone Marker M.wav</t>
-  </si>
-  <si>
-    <t>Male - Tone Marker D.wav</t>
-  </si>
-  <si>
-    <t>Male - Tone Marker (-).wav</t>
-  </si>
-  <si>
-    <t>Male - Single Vowel A.wav</t>
-  </si>
-  <si>
-    <t>Male - Single Vowel E.wav</t>
-  </si>
-  <si>
-    <t>Male - Single Vowel I.wav</t>
-  </si>
-  <si>
-    <t>Male - Single Vowel O.wav</t>
-  </si>
-  <si>
-    <t>Male - Single Vowel U.wav</t>
-  </si>
-  <si>
-    <t>Male - Single Vowel W.wav</t>
-  </si>
-  <si>
-    <t>Male - Double Vowel AI.wav</t>
-  </si>
-  <si>
-    <t>Male - Double Vowel AU.wav</t>
-  </si>
-  <si>
-    <t>Male - Double Vowel AW.wav</t>
-  </si>
-  <si>
-    <t>Male - Double Vowel EE.wav</t>
-  </si>
-  <si>
-    <t>Male - Double Vowel IA.wav</t>
-  </si>
-  <si>
-    <t>Male - Double Vowel OO.wav</t>
-  </si>
-  <si>
-    <t>Male - Double Vowel UA.wav</t>
-  </si>
-  <si>
-    <t>Male - Consonant C.wav</t>
-  </si>
-  <si>
-    <t>Male - Consonant D.wav</t>
-  </si>
-  <si>
-    <t>Male - Consonant F.wav</t>
-  </si>
-  <si>
-    <t>Male - Consonant H.wav</t>
-  </si>
-  <si>
-    <t>Male - Consonant K.wav</t>
-  </si>
-  <si>
-    <t>Male - Consonant L.wav</t>
-  </si>
-  <si>
-    <t>Male - Consonant M.wav</t>
-  </si>
-  <si>
-    <t>Male - Consonant N.wav</t>
-  </si>
-  <si>
-    <t>Male - Consonant P.wav</t>
-  </si>
-  <si>
-    <t>Male - Consonant Q.wav</t>
-  </si>
-  <si>
-    <t>Male - Consonant R.wav</t>
-  </si>
-  <si>
-    <t>Male - Consonant S.wav</t>
-  </si>
-  <si>
-    <t>Male - Consonant T.wav</t>
-  </si>
-  <si>
-    <t>Male - Consonant V.wav</t>
-  </si>
-  <si>
-    <t>Male - Consonant X.wav</t>
-  </si>
-  <si>
-    <t>Male - Consonant Y.wav</t>
-  </si>
-  <si>
-    <t>Male - Consonant Z.wav</t>
+    <t>Male - Single Consonant L.wav</t>
+  </si>
+  <si>
+    <t>Male - Single Consonant C.wav</t>
+  </si>
+  <si>
+    <t>Male - Single Consonant D.wav</t>
+  </si>
+  <si>
+    <t>Male - Single Consonant F.wav</t>
+  </si>
+  <si>
+    <t>Male - Single Consonant H.wav</t>
+  </si>
+  <si>
+    <t>Male - Single Consonant K.wav</t>
+  </si>
+  <si>
+    <t>Male - Single Consonant M.wav</t>
+  </si>
+  <si>
+    <t>Male - Single Consonant N.wav</t>
+  </si>
+  <si>
+    <t>Male - Single Consonant P.wav</t>
+  </si>
+  <si>
+    <t>Male - Single Consonant Q.wav</t>
+  </si>
+  <si>
+    <t>Male - Single Consonant R.wav</t>
+  </si>
+  <si>
+    <t>Male - Single Consonant S.wav</t>
+  </si>
+  <si>
+    <t>Male - Single Consonant T.wav</t>
+  </si>
+  <si>
+    <t>Male - Single Consonant V.wav</t>
+  </si>
+  <si>
+    <t>Male - Single Consonant X.wav</t>
+  </si>
+  <si>
+    <t>Male - Single Consonant Y.wav</t>
+  </si>
+  <si>
+    <t>Male - Single Consonant Z.wav</t>
+  </si>
+  <si>
+    <t>Female - Single Consonant Z.wav</t>
+  </si>
+  <si>
+    <t>Female - Single Consonant Y.wav</t>
+  </si>
+  <si>
+    <t>Female - Single Consonant X.wav</t>
+  </si>
+  <si>
+    <t>Female - Single Consonant V.wav</t>
+  </si>
+  <si>
+    <t>Female - Single Consonant S.wav</t>
+  </si>
+  <si>
+    <t>Female - Single Consonant R.wav</t>
+  </si>
+  <si>
+    <t>Female - Single Consonant P.wav</t>
+  </si>
+  <si>
+    <t>Female - Single Consonant M.wav</t>
+  </si>
+  <si>
+    <t>Female - Single Consonant K.wav</t>
+  </si>
+  <si>
+    <t>Female - Single Consonant F.wav</t>
+  </si>
+  <si>
+    <t>Female - Single Consonant C.wav</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -993,23 +993,34 @@
       <family val="2"/>
     </font>
     <font>
-      <sz val="11"/>
+      <b/>
+      <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <u/>
-      <sz val="11"/>
+      <sz val="12"/>
       <color rgb="FF0000FF"/>
       <name val="Calibri"/>
       <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Aptos"/>
-      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -1054,18 +1065,19 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -1375,8 +1387,8 @@
   </sheetPr>
   <dimension ref="A1:J1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C61" zoomScale="119" workbookViewId="0">
-      <selection activeCell="D74" sqref="D74"/>
+    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="A57" sqref="A57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1389,1337 +1401,1603 @@
     <col min="6" max="6" width="26.26953125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="14.453125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="20.54296875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="23.26953125" customWidth="1"/>
+    <col min="9" max="9" width="23.26953125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="23.7265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="I1" s="2" t="s">
         <v>8</v>
       </c>
       <c r="J1" s="1"/>
     </row>
     <row r="2" spans="1:10" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="E2" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="I2" t="s">
+      <c r="F2" s="4"/>
+      <c r="G2" s="4"/>
+      <c r="H2" s="4"/>
+      <c r="I2" s="4" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:10" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="2" t="s">
+      <c r="A3" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C3" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="D3" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="E3" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="I3" t="s">
+      <c r="F3" s="4"/>
+      <c r="G3" s="4"/>
+      <c r="H3" s="4"/>
+      <c r="I3" s="4" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="4" spans="1:10" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="2" t="s">
+      <c r="A4" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B4" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="C4" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="D4" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="E4" s="2" t="s">
+      <c r="E4" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="I4" t="s">
+      <c r="F4" s="4"/>
+      <c r="G4" s="4"/>
+      <c r="H4" s="4"/>
+      <c r="I4" s="4" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="5" spans="1:10" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="2" t="s">
+      <c r="A5" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="B5" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="C5" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="D5" s="3" t="s">
+      <c r="D5" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="E5" s="2" t="s">
+      <c r="E5" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="I5" t="s">
+      <c r="F5" s="4"/>
+      <c r="G5" s="4"/>
+      <c r="H5" s="4"/>
+      <c r="I5" s="4" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="6" spans="1:10" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="2" t="s">
+      <c r="A6" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="B6" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="C6" s="2" t="s">
+      <c r="C6" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="D6" s="2" t="s">
+      <c r="D6" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="E6" s="2" t="s">
+      <c r="E6" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="I6" t="s">
+      <c r="F6" s="4"/>
+      <c r="G6" s="4"/>
+      <c r="H6" s="4"/>
+      <c r="I6" s="4" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="7" spans="1:10" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="2" t="s">
+      <c r="A7" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="B7" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="C7" s="2" t="s">
+      <c r="C7" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="D7" s="2" t="s">
+      <c r="D7" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="E7" s="2" t="s">
+      <c r="E7" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="I7" t="s">
+      <c r="F7" s="4"/>
+      <c r="G7" s="4"/>
+      <c r="H7" s="4"/>
+      <c r="I7" s="4" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="8" spans="1:10" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="2" t="s">
+      <c r="A8" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="B8" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="C8" s="2" t="s">
+      <c r="C8" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="D8" s="2" t="s">
+      <c r="D8" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="E8" s="2" t="s">
+      <c r="E8" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="I8" t="s">
+      <c r="F8" s="4"/>
+      <c r="G8" s="4"/>
+      <c r="H8" s="4"/>
+      <c r="I8" s="4" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="9" spans="1:10" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="2" t="s">
+      <c r="A9" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="B9" s="2" t="s">
+      <c r="B9" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="C9" s="2" t="s">
+      <c r="C9" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="D9" s="2" t="s">
+      <c r="D9" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="E9" s="2" t="s">
+      <c r="E9" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="I9" t="s">
+      <c r="F9" s="4"/>
+      <c r="G9" s="4"/>
+      <c r="H9" s="4"/>
+      <c r="I9" s="4" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="10" spans="1:10" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="2" t="s">
+      <c r="A10" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="B10" s="2" t="s">
+      <c r="B10" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="C10" s="2" t="s">
+      <c r="C10" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="D10" s="2" t="s">
+      <c r="D10" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="E10" s="2" t="s">
+      <c r="E10" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="I10" t="s">
+      <c r="F10" s="4"/>
+      <c r="G10" s="4"/>
+      <c r="H10" s="4"/>
+      <c r="I10" s="4" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="11" spans="1:10" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="2" t="s">
+      <c r="A11" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="B11" s="2" t="s">
+      <c r="B11" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="C11" s="2" t="s">
+      <c r="C11" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="D11" s="2" t="s">
+      <c r="D11" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="E11" s="2" t="s">
+      <c r="E11" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="I11" t="s">
+      <c r="F11" s="4"/>
+      <c r="G11" s="4"/>
+      <c r="H11" s="4"/>
+      <c r="I11" s="4" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="12" spans="1:10" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="2" t="s">
+      <c r="A12" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="B12" s="2" t="s">
+      <c r="B12" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="C12" s="2" t="s">
+      <c r="C12" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="D12" s="2" t="s">
+      <c r="D12" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="E12" s="2" t="s">
+      <c r="E12" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="I12" t="s">
+      <c r="F12" s="4"/>
+      <c r="G12" s="4"/>
+      <c r="H12" s="4"/>
+      <c r="I12" s="4" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="13" spans="1:10" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="2" t="s">
+      <c r="A13" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="B13" s="2" t="s">
+      <c r="B13" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="C13" s="2" t="s">
+      <c r="C13" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="D13" s="2" t="s">
+      <c r="D13" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="E13" s="2" t="s">
+      <c r="E13" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="I13" t="s">
+      <c r="F13" s="4"/>
+      <c r="G13" s="4"/>
+      <c r="H13" s="4"/>
+      <c r="I13" s="4" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="14" spans="1:10" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="2" t="s">
+      <c r="A14" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="B14" s="2" t="s">
+      <c r="B14" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="C14" s="2" t="s">
+      <c r="C14" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="D14" s="2" t="s">
+      <c r="D14" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="E14" s="2" t="s">
+      <c r="E14" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="I14" t="s">
+      <c r="F14" s="4"/>
+      <c r="G14" s="4"/>
+      <c r="H14" s="4"/>
+      <c r="I14" s="4" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="15" spans="1:10" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="2" t="s">
+      <c r="A15" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="B15" s="2" t="s">
+      <c r="B15" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="C15" s="2" t="s">
+      <c r="C15" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="D15" s="2" t="s">
+      <c r="D15" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="E15" s="2" t="s">
+      <c r="E15" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="I15" t="s">
+      <c r="F15" s="4"/>
+      <c r="G15" s="4"/>
+      <c r="H15" s="4"/>
+      <c r="I15" s="4" t="s">
         <v>80</v>
       </c>
     </row>
     <row r="16" spans="1:10" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="2" t="s">
+      <c r="A16" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="B16" s="2" t="s">
+      <c r="B16" s="3" t="s">
         <v>82</v>
       </c>
-      <c r="C16" s="2" t="s">
+      <c r="C16" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="D16" s="2" t="s">
+      <c r="D16" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="E16" s="2" t="s">
+      <c r="E16" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="I16" t="s">
+      <c r="F16" s="4"/>
+      <c r="G16" s="4"/>
+      <c r="H16" s="4"/>
+      <c r="I16" s="4" t="s">
         <v>85</v>
       </c>
     </row>
     <row r="17" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="2" t="s">
+      <c r="A17" s="3" t="s">
         <v>86</v>
       </c>
-      <c r="B17" s="2" t="s">
+      <c r="B17" s="3" t="s">
         <v>87</v>
       </c>
-      <c r="C17" s="2" t="s">
+      <c r="C17" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="D17" s="2" t="s">
+      <c r="D17" s="3" t="s">
         <v>88</v>
       </c>
-      <c r="E17" s="2" t="s">
+      <c r="E17" s="3" t="s">
         <v>89</v>
       </c>
-      <c r="I17" t="s">
+      <c r="F17" s="4"/>
+      <c r="G17" s="4"/>
+      <c r="H17" s="4"/>
+      <c r="I17" s="4" t="s">
         <v>90</v>
       </c>
     </row>
     <row r="18" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="2" t="s">
+      <c r="A18" s="3" t="s">
         <v>91</v>
       </c>
-      <c r="B18" s="2" t="s">
+      <c r="B18" s="3" t="s">
         <v>92</v>
       </c>
-      <c r="C18" s="2" t="s">
+      <c r="C18" s="3" t="s">
         <v>93</v>
       </c>
-      <c r="D18" s="2" t="s">
+      <c r="D18" s="3" t="s">
         <v>94</v>
       </c>
-      <c r="E18" s="2" t="s">
+      <c r="E18" s="3" t="s">
         <v>95</v>
       </c>
+      <c r="F18" s="4"/>
+      <c r="G18" s="4"/>
+      <c r="H18" s="4"/>
+      <c r="I18" s="4"/>
     </row>
     <row r="19" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="2" t="s">
+      <c r="A19" s="3" t="s">
         <v>96</v>
       </c>
-      <c r="B19" s="2" t="s">
+      <c r="B19" s="3" t="s">
         <v>97</v>
       </c>
-      <c r="C19" s="2" t="s">
+      <c r="C19" s="3" t="s">
         <v>93</v>
       </c>
-      <c r="D19" s="2" t="s">
+      <c r="D19" s="3" t="s">
         <v>98</v>
       </c>
-      <c r="E19" s="2" t="s">
+      <c r="E19" s="3" t="s">
         <v>99</v>
       </c>
+      <c r="F19" s="4"/>
+      <c r="G19" s="4"/>
+      <c r="H19" s="4"/>
+      <c r="I19" s="4"/>
     </row>
     <row r="20" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="2" t="s">
+      <c r="A20" s="3" t="s">
         <v>100</v>
       </c>
-      <c r="B20" s="2" t="s">
+      <c r="B20" s="3" t="s">
         <v>101</v>
       </c>
-      <c r="C20" s="2" t="s">
+      <c r="C20" s="3" t="s">
         <v>93</v>
       </c>
-      <c r="D20" s="2" t="s">
+      <c r="D20" s="3" t="s">
         <v>102</v>
       </c>
-      <c r="E20" s="2" t="s">
+      <c r="E20" s="3" t="s">
         <v>103</v>
       </c>
+      <c r="F20" s="4"/>
+      <c r="G20" s="4"/>
+      <c r="H20" s="4"/>
+      <c r="I20" s="4"/>
     </row>
     <row r="21" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="2" t="s">
+      <c r="A21" s="3" t="s">
         <v>104</v>
       </c>
-      <c r="B21" s="2" t="s">
+      <c r="B21" s="3" t="s">
         <v>105</v>
       </c>
-      <c r="C21" s="2" t="s">
+      <c r="C21" s="3" t="s">
         <v>93</v>
       </c>
-      <c r="D21" s="2" t="s">
+      <c r="D21" s="3" t="s">
         <v>106</v>
       </c>
-      <c r="E21" s="2" t="s">
+      <c r="E21" s="3" t="s">
         <v>107</v>
       </c>
+      <c r="F21" s="4"/>
+      <c r="G21" s="4"/>
+      <c r="H21" s="4"/>
+      <c r="I21" s="4"/>
     </row>
     <row r="22" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="2" t="s">
+      <c r="A22" s="3" t="s">
         <v>108</v>
       </c>
-      <c r="B22" s="2" t="s">
+      <c r="B22" s="3" t="s">
         <v>109</v>
       </c>
-      <c r="C22" s="2" t="s">
+      <c r="C22" s="3" t="s">
         <v>110</v>
       </c>
-      <c r="D22" s="2" t="s">
+      <c r="D22" s="3" t="s">
         <v>111</v>
       </c>
-      <c r="E22" s="2" t="s">
+      <c r="E22" s="3" t="s">
         <v>112</v>
       </c>
-      <c r="I22" t="s">
+      <c r="F22" s="4"/>
+      <c r="G22" s="4"/>
+      <c r="H22" s="4"/>
+      <c r="I22" s="4" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A23" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="C23" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="D23" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="E23" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="F23" s="4"/>
+      <c r="G23" s="4"/>
+      <c r="H23" s="4"/>
+      <c r="I23" s="4" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A24" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="B24" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="C24" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="D24" s="4"/>
+      <c r="E24" s="3" t="s">
+        <v>121</v>
+      </c>
+      <c r="F24" s="4"/>
+      <c r="G24" s="4"/>
+      <c r="H24" s="4"/>
+      <c r="I24" s="4" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A25" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="B25" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="C25" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="D25" s="4"/>
+      <c r="E25" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="F25" s="4"/>
+      <c r="G25" s="4"/>
+      <c r="H25" s="4"/>
+      <c r="I25" s="4" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A26" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="B26" s="3" t="s">
+        <v>128</v>
+      </c>
+      <c r="C26" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="D26" s="4"/>
+      <c r="E26" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="F26" s="4"/>
+      <c r="G26" s="4"/>
+      <c r="H26" s="4"/>
+      <c r="I26" s="4" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A27" s="3" t="s">
+        <v>131</v>
+      </c>
+      <c r="B27" s="3" t="s">
+        <v>132</v>
+      </c>
+      <c r="C27" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="D27" s="4"/>
+      <c r="E27" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="F27" s="4"/>
+      <c r="G27" s="4"/>
+      <c r="H27" s="4"/>
+      <c r="I27" s="4" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A28" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="B28" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="C28" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="D28" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="E28" s="4"/>
+      <c r="F28" s="4"/>
+      <c r="G28" s="4"/>
+      <c r="H28" s="4"/>
+      <c r="I28" s="4" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A29" s="3" t="s">
+        <v>138</v>
+      </c>
+      <c r="B29" s="3" t="s">
+        <v>139</v>
+      </c>
+      <c r="C29" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="D29" s="3" t="s">
+        <v>140</v>
+      </c>
+      <c r="E29" s="4"/>
+      <c r="F29" s="4"/>
+      <c r="G29" s="4"/>
+      <c r="H29" s="4"/>
+      <c r="I29" s="4" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A30" s="3" t="s">
+        <v>141</v>
+      </c>
+      <c r="B30" s="3" t="s">
+        <v>142</v>
+      </c>
+      <c r="C30" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="D30" s="3" t="s">
+        <v>143</v>
+      </c>
+      <c r="E30" s="4"/>
+      <c r="F30" s="4"/>
+      <c r="G30" s="4"/>
+      <c r="H30" s="4"/>
+      <c r="I30" s="4" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A31" s="3" t="s">
+        <v>144</v>
+      </c>
+      <c r="B31" s="3" t="s">
+        <v>145</v>
+      </c>
+      <c r="C31" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="D31" s="3" t="s">
+        <v>146</v>
+      </c>
+      <c r="E31" s="4"/>
+      <c r="F31" s="4"/>
+      <c r="G31" s="4"/>
+      <c r="H31" s="4"/>
+      <c r="I31" s="4" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A32" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="B32" s="3" t="s">
+        <v>148</v>
+      </c>
+      <c r="C32" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="D32" s="3" t="s">
+        <v>149</v>
+      </c>
+      <c r="E32" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="F32" s="4"/>
+      <c r="G32" s="4"/>
+      <c r="H32" s="4"/>
+      <c r="I32" s="4" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A33" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="B33" s="3" t="s">
+        <v>153</v>
+      </c>
+      <c r="C33" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="D33" s="3" t="s">
+        <v>154</v>
+      </c>
+      <c r="E33" s="3" t="s">
+        <v>155</v>
+      </c>
+      <c r="F33" s="4"/>
+      <c r="G33" s="4"/>
+      <c r="H33" s="4"/>
+      <c r="I33" s="4" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A34" s="3" t="s">
+        <v>157</v>
+      </c>
+      <c r="B34" s="3" t="s">
+        <v>158</v>
+      </c>
+      <c r="C34" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="D34" s="3" t="s">
+        <v>159</v>
+      </c>
+      <c r="E34" s="3" t="s">
+        <v>160</v>
+      </c>
+      <c r="F34" s="4"/>
+      <c r="G34" s="4"/>
+      <c r="H34" s="4"/>
+      <c r="I34" s="4" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A35" s="3" t="s">
+        <v>162</v>
+      </c>
+      <c r="B35" s="3" t="s">
+        <v>163</v>
+      </c>
+      <c r="C35" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="D35" s="3" t="s">
+        <v>164</v>
+      </c>
+      <c r="E35" s="3" t="s">
+        <v>165</v>
+      </c>
+      <c r="F35" s="4"/>
+      <c r="G35" s="4"/>
+      <c r="H35" s="4"/>
+      <c r="I35" s="4" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A36" s="4" t="s">
+        <v>167</v>
+      </c>
+      <c r="B36" s="4" t="s">
+        <v>168</v>
+      </c>
+      <c r="C36" s="4" t="s">
+        <v>169</v>
+      </c>
+      <c r="D36" s="4" t="s">
+        <v>170</v>
+      </c>
+      <c r="E36" s="3" t="s">
+        <v>171</v>
+      </c>
+      <c r="F36" s="4"/>
+      <c r="G36" s="4"/>
+      <c r="H36" s="4"/>
+      <c r="I36" s="4"/>
+    </row>
+    <row r="37" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A37" s="4" t="s">
+        <v>172</v>
+      </c>
+      <c r="B37" s="4" t="s">
+        <v>173</v>
+      </c>
+      <c r="C37" s="4" t="s">
+        <v>169</v>
+      </c>
+      <c r="D37" s="4" t="s">
+        <v>174</v>
+      </c>
+      <c r="E37" s="3" t="s">
+        <v>175</v>
+      </c>
+      <c r="F37" s="4"/>
+      <c r="G37" s="4"/>
+      <c r="H37" s="4"/>
+      <c r="I37" s="4"/>
+    </row>
+    <row r="38" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A38" s="4" t="s">
+        <v>176</v>
+      </c>
+      <c r="B38" s="4" t="s">
+        <v>177</v>
+      </c>
+      <c r="C38" s="4" t="s">
+        <v>169</v>
+      </c>
+      <c r="D38" s="4" t="s">
+        <v>178</v>
+      </c>
+      <c r="E38" s="3" t="s">
+        <v>179</v>
+      </c>
+      <c r="F38" s="4"/>
+      <c r="G38" s="4"/>
+      <c r="H38" s="4"/>
+      <c r="I38" s="4"/>
+    </row>
+    <row r="39" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A39" s="4" t="s">
+        <v>180</v>
+      </c>
+      <c r="B39" s="4" t="s">
+        <v>181</v>
+      </c>
+      <c r="C39" s="4" t="s">
+        <v>169</v>
+      </c>
+      <c r="D39" s="4" t="s">
+        <v>182</v>
+      </c>
+      <c r="E39" s="3" t="s">
+        <v>183</v>
+      </c>
+      <c r="F39" s="4"/>
+      <c r="G39" s="4"/>
+      <c r="H39" s="4"/>
+      <c r="I39" s="4"/>
+    </row>
+    <row r="40" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A40" s="4" t="s">
+        <v>184</v>
+      </c>
+      <c r="B40" s="4" t="s">
+        <v>185</v>
+      </c>
+      <c r="C40" s="4" t="s">
+        <v>169</v>
+      </c>
+      <c r="D40" s="4" t="s">
+        <v>186</v>
+      </c>
+      <c r="E40" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="F40" s="4"/>
+      <c r="G40" s="4"/>
+      <c r="H40" s="4"/>
+      <c r="I40" s="4"/>
+    </row>
+    <row r="41" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A41" s="4" t="s">
+        <v>188</v>
+      </c>
+      <c r="B41" s="4" t="s">
+        <v>189</v>
+      </c>
+      <c r="C41" s="4" t="s">
+        <v>169</v>
+      </c>
+      <c r="D41" s="4" t="s">
+        <v>190</v>
+      </c>
+      <c r="E41" s="3" t="s">
+        <v>191</v>
+      </c>
+      <c r="F41" s="4"/>
+      <c r="G41" s="4"/>
+      <c r="H41" s="4"/>
+      <c r="I41" s="4"/>
+    </row>
+    <row r="42" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A42" s="4" t="s">
+        <v>192</v>
+      </c>
+      <c r="B42" s="4" t="s">
+        <v>193</v>
+      </c>
+      <c r="C42" s="4" t="s">
+        <v>169</v>
+      </c>
+      <c r="D42" s="4" t="s">
+        <v>194</v>
+      </c>
+      <c r="E42" s="3" t="s">
+        <v>195</v>
+      </c>
+      <c r="F42" s="4"/>
+      <c r="G42" s="4"/>
+      <c r="H42" s="4"/>
+      <c r="I42" s="4"/>
+    </row>
+    <row r="43" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A43" s="3" t="s">
+        <v>196</v>
+      </c>
+      <c r="B43" s="4" t="s">
+        <v>197</v>
+      </c>
+      <c r="C43" s="4" t="s">
+        <v>169</v>
+      </c>
+      <c r="D43" s="4" t="s">
+        <v>198</v>
+      </c>
+      <c r="E43" s="3" t="s">
+        <v>199</v>
+      </c>
+      <c r="F43" s="4"/>
+      <c r="G43" s="4"/>
+      <c r="H43" s="4"/>
+      <c r="I43" s="4"/>
+    </row>
+    <row r="44" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A44" s="4" t="s">
+        <v>200</v>
+      </c>
+      <c r="B44" s="4" t="s">
+        <v>201</v>
+      </c>
+      <c r="C44" s="4" t="s">
+        <v>202</v>
+      </c>
+      <c r="D44" s="4" t="s">
+        <v>203</v>
+      </c>
+      <c r="E44" s="3" t="s">
+        <v>204</v>
+      </c>
+      <c r="F44" s="4"/>
+      <c r="G44" s="4"/>
+      <c r="H44" s="4"/>
+      <c r="I44" s="4"/>
+    </row>
+    <row r="45" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A45" s="4" t="s">
+        <v>205</v>
+      </c>
+      <c r="B45" s="4" t="s">
+        <v>206</v>
+      </c>
+      <c r="C45" s="4" t="s">
+        <v>202</v>
+      </c>
+      <c r="D45" s="4" t="s">
+        <v>207</v>
+      </c>
+      <c r="E45" s="3" t="s">
+        <v>208</v>
+      </c>
+      <c r="F45" s="4"/>
+      <c r="G45" s="4"/>
+      <c r="H45" s="4"/>
+      <c r="I45" s="4"/>
+    </row>
+    <row r="46" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A46" s="4" t="s">
+        <v>209</v>
+      </c>
+      <c r="B46" s="4" t="s">
+        <v>210</v>
+      </c>
+      <c r="C46" s="4" t="s">
+        <v>202</v>
+      </c>
+      <c r="D46" s="4" t="s">
+        <v>211</v>
+      </c>
+      <c r="E46" s="3" t="s">
+        <v>212</v>
+      </c>
+      <c r="F46" s="4"/>
+      <c r="G46" s="4"/>
+      <c r="H46" s="4"/>
+      <c r="I46" s="4"/>
+    </row>
+    <row r="47" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A47" s="4" t="s">
+        <v>213</v>
+      </c>
+      <c r="B47" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C47" s="4" t="s">
+        <v>202</v>
+      </c>
+      <c r="D47" s="4" t="s">
+        <v>214</v>
+      </c>
+      <c r="E47" s="3" t="s">
+        <v>215</v>
+      </c>
+      <c r="F47" s="4"/>
+      <c r="G47" s="4"/>
+      <c r="H47" s="4"/>
+      <c r="I47" s="4"/>
+    </row>
+    <row r="48" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A48" s="4" t="s">
+        <v>216</v>
+      </c>
+      <c r="B48" s="4" t="s">
+        <v>217</v>
+      </c>
+      <c r="C48" s="4" t="s">
+        <v>202</v>
+      </c>
+      <c r="D48" s="4" t="s">
+        <v>218</v>
+      </c>
+      <c r="E48" s="3" t="s">
+        <v>219</v>
+      </c>
+      <c r="F48" s="4"/>
+      <c r="G48" s="4"/>
+      <c r="H48" s="4"/>
+      <c r="I48" s="4"/>
+    </row>
+    <row r="49" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A49" s="4" t="s">
+        <v>220</v>
+      </c>
+      <c r="B49" s="4" t="s">
+        <v>221</v>
+      </c>
+      <c r="C49" s="4" t="s">
+        <v>202</v>
+      </c>
+      <c r="D49" s="4" t="s">
+        <v>222</v>
+      </c>
+      <c r="E49" s="3" t="s">
+        <v>223</v>
+      </c>
+      <c r="F49" s="4"/>
+      <c r="G49" s="4"/>
+      <c r="H49" s="4"/>
+      <c r="I49" s="4"/>
+    </row>
+    <row r="50" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A50" s="4" t="s">
+        <v>224</v>
+      </c>
+      <c r="B50" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="C50" s="4" t="s">
+        <v>225</v>
+      </c>
+      <c r="D50" s="4" t="s">
+        <v>226</v>
+      </c>
+      <c r="E50" s="3" t="s">
+        <v>227</v>
+      </c>
+      <c r="F50" s="4"/>
+      <c r="G50" s="4"/>
+      <c r="H50" s="4"/>
+      <c r="I50" s="4"/>
+    </row>
+    <row r="51" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A51" s="4" t="s">
+        <v>228</v>
+      </c>
+      <c r="B51" s="4" t="s">
+        <v>229</v>
+      </c>
+      <c r="C51" s="4" t="s">
+        <v>225</v>
+      </c>
+      <c r="D51" s="4" t="s">
+        <v>230</v>
+      </c>
+      <c r="E51" s="3" t="s">
         <v>231</v>
       </c>
-    </row>
-    <row r="23" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A23" s="2" t="s">
-        <v>113</v>
-      </c>
-      <c r="B23" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="C23" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="D23" s="2" t="s">
-        <v>115</v>
-      </c>
-      <c r="E23" s="2" t="s">
-        <v>116</v>
-      </c>
-      <c r="I23" t="s">
+      <c r="F51" s="4"/>
+      <c r="G51" s="4"/>
+      <c r="H51" s="4"/>
+      <c r="I51" s="4"/>
+    </row>
+    <row r="52" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A52" s="4" t="s">
         <v>232</v>
       </c>
-    </row>
-    <row r="24" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A24" s="2" t="s">
-        <v>117</v>
-      </c>
-      <c r="B24" s="2" t="s">
-        <v>118</v>
-      </c>
-      <c r="C24" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="E24" s="2" t="s">
-        <v>119</v>
-      </c>
-      <c r="I24" t="s">
+      <c r="B52" s="4" t="s">
         <v>233</v>
       </c>
-    </row>
-    <row r="25" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A25" s="2" t="s">
-        <v>120</v>
-      </c>
-      <c r="B25" s="2" t="s">
-        <v>121</v>
-      </c>
-      <c r="C25" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="E25" s="2" t="s">
-        <v>122</v>
-      </c>
-      <c r="I25" t="s">
+      <c r="C52" s="4" t="s">
+        <v>225</v>
+      </c>
+      <c r="D52" s="4" t="s">
         <v>234</v>
       </c>
-    </row>
-    <row r="26" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A26" s="2" t="s">
-        <v>123</v>
-      </c>
-      <c r="B26" s="2" t="s">
-        <v>124</v>
-      </c>
-      <c r="C26" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="E26" s="2" t="s">
-        <v>125</v>
-      </c>
-      <c r="I26" t="s">
+      <c r="E52" s="3" t="s">
         <v>235</v>
       </c>
-    </row>
-    <row r="27" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A27" s="2" t="s">
-        <v>126</v>
-      </c>
-      <c r="B27" s="2" t="s">
-        <v>127</v>
-      </c>
-      <c r="C27" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="E27" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="I27" t="s">
+      <c r="F52" s="4"/>
+      <c r="G52" s="4"/>
+      <c r="H52" s="4"/>
+      <c r="I52" s="4"/>
+    </row>
+    <row r="53" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A53" s="4" t="s">
         <v>236</v>
       </c>
-    </row>
-    <row r="28" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A28" s="2" t="s">
-        <v>129</v>
-      </c>
-      <c r="B28" s="2" t="s">
-        <v>130</v>
-      </c>
-      <c r="C28" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="D28" s="2" t="s">
-        <v>131</v>
-      </c>
-      <c r="I28" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="29" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A29" s="2" t="s">
-        <v>132</v>
-      </c>
-      <c r="B29" s="2" t="s">
-        <v>133</v>
-      </c>
-      <c r="C29" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="D29" s="2" t="s">
-        <v>134</v>
-      </c>
-      <c r="I29" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="30" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A30" s="2" t="s">
-        <v>135</v>
-      </c>
-      <c r="B30" s="2" t="s">
-        <v>136</v>
-      </c>
-      <c r="C30" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="D30" s="2" t="s">
-        <v>137</v>
-      </c>
-      <c r="I30" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="31" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A31" s="2" t="s">
-        <v>138</v>
-      </c>
-      <c r="B31" s="2" t="s">
-        <v>139</v>
-      </c>
-      <c r="C31" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="D31" s="2" t="s">
-        <v>140</v>
-      </c>
-      <c r="I31" t="s">
-        <v>236</v>
-      </c>
-    </row>
-    <row r="32" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A32" s="2" t="s">
-        <v>141</v>
-      </c>
-      <c r="B32" s="2" t="s">
-        <v>142</v>
-      </c>
-      <c r="C32" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="D32" s="2" t="s">
-        <v>143</v>
-      </c>
-      <c r="E32" s="2" t="s">
-        <v>144</v>
-      </c>
-      <c r="I32" t="s">
+      <c r="B53" s="4" t="s">
         <v>237</v>
       </c>
-    </row>
-    <row r="33" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A33" s="2" t="s">
-        <v>145</v>
-      </c>
-      <c r="B33" s="2" t="s">
-        <v>146</v>
-      </c>
-      <c r="C33" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="D33" s="2" t="s">
-        <v>147</v>
-      </c>
-      <c r="E33" s="2" t="s">
-        <v>148</v>
-      </c>
-      <c r="I33" t="s">
+      <c r="C53" s="4" t="s">
+        <v>225</v>
+      </c>
+      <c r="D53" s="4" t="s">
         <v>238</v>
       </c>
-    </row>
-    <row r="34" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A34" s="2" t="s">
-        <v>149</v>
-      </c>
-      <c r="B34" s="2" t="s">
-        <v>150</v>
-      </c>
-      <c r="C34" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="D34" s="2" t="s">
-        <v>151</v>
-      </c>
-      <c r="E34" s="2" t="s">
-        <v>152</v>
-      </c>
-      <c r="I34" t="s">
+      <c r="E53" s="3" t="s">
         <v>239</v>
       </c>
-    </row>
-    <row r="35" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A35" s="2" t="s">
-        <v>153</v>
-      </c>
-      <c r="B35" s="2" t="s">
-        <v>154</v>
-      </c>
-      <c r="C35" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="D35" s="2" t="s">
-        <v>155</v>
-      </c>
-      <c r="E35" s="2" t="s">
-        <v>156</v>
-      </c>
-      <c r="I35" t="s">
+      <c r="F53" s="4"/>
+      <c r="G53" s="4"/>
+      <c r="H53" s="4"/>
+      <c r="I53" s="4"/>
+    </row>
+    <row r="54" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A54" s="4" t="s">
         <v>240</v>
       </c>
-    </row>
-    <row r="36" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A36" t="s">
-        <v>157</v>
-      </c>
-      <c r="B36" t="s">
-        <v>158</v>
-      </c>
-      <c r="C36" t="s">
-        <v>159</v>
-      </c>
-      <c r="D36" t="s">
+      <c r="B54" s="4" t="s">
+        <v>241</v>
+      </c>
+      <c r="C54" s="4" t="s">
+        <v>225</v>
+      </c>
+      <c r="D54" s="4" t="s">
+        <v>242</v>
+      </c>
+      <c r="E54" s="3" t="s">
+        <v>243</v>
+      </c>
+      <c r="F54" s="4"/>
+      <c r="G54" s="4"/>
+      <c r="H54" s="4"/>
+      <c r="I54" s="4"/>
+    </row>
+    <row r="55" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A55" s="4" t="s">
+        <v>244</v>
+      </c>
+      <c r="B55" s="4" t="s">
+        <v>245</v>
+      </c>
+      <c r="C55" s="4" t="s">
+        <v>225</v>
+      </c>
+      <c r="D55" s="4" t="s">
+        <v>246</v>
+      </c>
+      <c r="E55" s="3" t="s">
+        <v>247</v>
+      </c>
+      <c r="F55" s="4"/>
+      <c r="G55" s="4"/>
+      <c r="H55" s="4"/>
+      <c r="I55" s="4"/>
+    </row>
+    <row r="56" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A56" s="4" t="s">
+        <v>248</v>
+      </c>
+      <c r="B56" s="4" t="s">
+        <v>249</v>
+      </c>
+      <c r="C56" s="4" t="s">
+        <v>225</v>
+      </c>
+      <c r="D56" s="4" t="s">
+        <v>250</v>
+      </c>
+      <c r="E56" s="3" t="s">
+        <v>251</v>
+      </c>
+      <c r="F56" s="4"/>
+      <c r="G56" s="4"/>
+      <c r="H56" s="4"/>
+      <c r="I56" s="4"/>
+    </row>
+    <row r="57" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A57" s="4" t="s">
+        <v>252</v>
+      </c>
+      <c r="B57" s="4" t="s">
+        <v>253</v>
+      </c>
+      <c r="C57" s="4" t="s">
+        <v>254</v>
+      </c>
+      <c r="D57" s="4" t="s">
+        <v>290</v>
+      </c>
+      <c r="E57" s="3" t="s">
+        <v>316</v>
+      </c>
+      <c r="F57" s="4"/>
+      <c r="G57" s="4"/>
+      <c r="H57" s="4"/>
+      <c r="I57" s="4"/>
+    </row>
+    <row r="58" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A58" s="4" t="s">
+        <v>192</v>
+      </c>
+      <c r="B58" s="4" t="s">
+        <v>255</v>
+      </c>
+      <c r="C58" s="4" t="s">
+        <v>254</v>
+      </c>
+      <c r="D58" s="4" t="s">
+        <v>291</v>
+      </c>
+      <c r="E58" s="3" t="s">
+        <v>256</v>
+      </c>
+      <c r="F58" s="4"/>
+      <c r="G58" s="4"/>
+      <c r="H58" s="4"/>
+      <c r="I58" s="4"/>
+    </row>
+    <row r="59" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A59" s="4" t="s">
+        <v>257</v>
+      </c>
+      <c r="B59" s="4" t="s">
+        <v>258</v>
+      </c>
+      <c r="C59" s="4" t="s">
+        <v>254</v>
+      </c>
+      <c r="D59" s="4" t="s">
+        <v>292</v>
+      </c>
+      <c r="E59" s="3" t="s">
+        <v>315</v>
+      </c>
+      <c r="F59" s="4"/>
+      <c r="G59" s="4"/>
+      <c r="H59" s="4"/>
+      <c r="I59" s="4"/>
+    </row>
+    <row r="60" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A60" s="4" t="s">
+        <v>259</v>
+      </c>
+      <c r="B60" s="4" t="s">
+        <v>260</v>
+      </c>
+      <c r="C60" s="4" t="s">
+        <v>254</v>
+      </c>
+      <c r="D60" s="4" t="s">
+        <v>293</v>
+      </c>
+      <c r="E60" s="3" t="s">
+        <v>261</v>
+      </c>
+      <c r="F60" s="4"/>
+      <c r="G60" s="4"/>
+      <c r="H60" s="4"/>
+      <c r="I60" s="4"/>
+    </row>
+    <row r="61" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A61" s="4" t="s">
+        <v>262</v>
+      </c>
+      <c r="B61" s="4" t="s">
+        <v>263</v>
+      </c>
+      <c r="C61" s="4" t="s">
+        <v>254</v>
+      </c>
+      <c r="D61" s="4" t="s">
+        <v>294</v>
+      </c>
+      <c r="E61" s="3" t="s">
+        <v>314</v>
+      </c>
+      <c r="F61" s="4"/>
+      <c r="G61" s="4"/>
+      <c r="H61" s="4"/>
+      <c r="I61" s="4"/>
+    </row>
+    <row r="62" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A62" s="4" t="s">
+        <v>264</v>
+      </c>
+      <c r="B62" s="4" t="s">
+        <v>265</v>
+      </c>
+      <c r="C62" s="4" t="s">
+        <v>254</v>
+      </c>
+      <c r="D62" s="4" t="s">
+        <v>289</v>
+      </c>
+      <c r="E62" s="3" t="s">
+        <v>266</v>
+      </c>
+      <c r="F62" s="4"/>
+      <c r="G62" s="4"/>
+      <c r="H62" s="4"/>
+      <c r="I62" s="4"/>
+    </row>
+    <row r="63" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A63" s="4" t="s">
+        <v>188</v>
+      </c>
+      <c r="B63" s="4" t="s">
+        <v>267</v>
+      </c>
+      <c r="C63" s="4" t="s">
+        <v>254</v>
+      </c>
+      <c r="D63" s="4" t="s">
+        <v>295</v>
+      </c>
+      <c r="E63" s="3" t="s">
+        <v>313</v>
+      </c>
+      <c r="F63" s="4"/>
+      <c r="G63" s="4"/>
+      <c r="H63" s="4"/>
+      <c r="I63" s="4"/>
+    </row>
+    <row r="64" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A64" s="4" t="s">
+        <v>268</v>
+      </c>
+      <c r="B64" s="4" t="s">
+        <v>269</v>
+      </c>
+      <c r="C64" s="4" t="s">
+        <v>254</v>
+      </c>
+      <c r="D64" s="4" t="s">
+        <v>296</v>
+      </c>
+      <c r="E64" s="3" t="s">
+        <v>270</v>
+      </c>
+      <c r="F64" s="4"/>
+      <c r="G64" s="4"/>
+      <c r="H64" s="4"/>
+      <c r="I64" s="4"/>
+    </row>
+    <row r="65" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A65" s="4" t="s">
+        <v>271</v>
+      </c>
+      <c r="B65" s="4" t="s">
+        <v>272</v>
+      </c>
+      <c r="C65" s="4" t="s">
+        <v>254</v>
+      </c>
+      <c r="D65" s="4" t="s">
+        <v>297</v>
+      </c>
+      <c r="E65" s="3" t="s">
+        <v>312</v>
+      </c>
+      <c r="F65" s="4"/>
+      <c r="G65" s="4"/>
+      <c r="H65" s="4"/>
+      <c r="I65" s="4"/>
+    </row>
+    <row r="66" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A66" s="4" t="s">
+        <v>273</v>
+      </c>
+      <c r="B66" s="4" t="s">
+        <v>274</v>
+      </c>
+      <c r="C66" s="4" t="s">
+        <v>254</v>
+      </c>
+      <c r="D66" s="4" t="s">
+        <v>298</v>
+      </c>
+      <c r="E66" s="3" t="s">
+        <v>275</v>
+      </c>
+      <c r="F66" s="4"/>
+      <c r="G66" s="4"/>
+      <c r="H66" s="4"/>
+      <c r="I66" s="4"/>
+    </row>
+    <row r="67" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A67" s="4" t="s">
+        <v>276</v>
+      </c>
+      <c r="B67" s="4" t="s">
+        <v>277</v>
+      </c>
+      <c r="C67" s="4" t="s">
+        <v>254</v>
+      </c>
+      <c r="D67" s="4" t="s">
+        <v>299</v>
+      </c>
+      <c r="E67" s="3" t="s">
+        <v>311</v>
+      </c>
+      <c r="F67" s="4"/>
+      <c r="G67" s="4"/>
+      <c r="H67" s="4"/>
+      <c r="I67" s="4"/>
+    </row>
+    <row r="68" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A68" s="4" t="s">
+        <v>180</v>
+      </c>
+      <c r="B68" s="4" t="s">
+        <v>278</v>
+      </c>
+      <c r="C68" s="4" t="s">
+        <v>254</v>
+      </c>
+      <c r="D68" s="4" t="s">
+        <v>300</v>
+      </c>
+      <c r="E68" s="3" t="s">
+        <v>310</v>
+      </c>
+      <c r="F68" s="4"/>
+      <c r="G68" s="4"/>
+      <c r="H68" s="4"/>
+      <c r="I68" s="4"/>
+    </row>
+    <row r="69" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A69" s="4" t="s">
         <v>279</v>
       </c>
-      <c r="E36" s="4" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="37" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A37" t="s">
-        <v>160</v>
-      </c>
-      <c r="B37" t="s">
-        <v>161</v>
-      </c>
-      <c r="C37" t="s">
-        <v>159</v>
-      </c>
-      <c r="D37" t="s">
+      <c r="B69" s="4" t="s">
         <v>280</v>
       </c>
-      <c r="E37" s="4" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="38" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A38" t="s">
-        <v>162</v>
-      </c>
-      <c r="B38" t="s">
-        <v>163</v>
-      </c>
-      <c r="C38" t="s">
-        <v>159</v>
-      </c>
-      <c r="D38" t="s">
+      <c r="C69" s="4" t="s">
+        <v>254</v>
+      </c>
+      <c r="D69" s="4" t="s">
+        <v>301</v>
+      </c>
+      <c r="E69" s="3" t="s">
         <v>281</v>
       </c>
-      <c r="E38" s="4" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="39" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A39" t="s">
-        <v>164</v>
-      </c>
-      <c r="B39" t="s">
-        <v>165</v>
-      </c>
-      <c r="C39" t="s">
-        <v>159</v>
-      </c>
-      <c r="D39" t="s">
+      <c r="F69" s="4"/>
+      <c r="G69" s="4"/>
+      <c r="H69" s="4"/>
+      <c r="I69" s="4"/>
+    </row>
+    <row r="70" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A70" s="4" t="s">
+        <v>176</v>
+      </c>
+      <c r="B70" s="4" t="s">
         <v>282</v>
       </c>
-      <c r="E39" s="4" t="s">
-        <v>253</v>
-      </c>
-    </row>
-    <row r="40" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A40" t="s">
-        <v>166</v>
-      </c>
-      <c r="B40" t="s">
-        <v>167</v>
-      </c>
-      <c r="C40" t="s">
-        <v>159</v>
-      </c>
-      <c r="D40" t="s">
+      <c r="C70" s="4" t="s">
+        <v>254</v>
+      </c>
+      <c r="D70" s="4" t="s">
+        <v>302</v>
+      </c>
+      <c r="E70" s="3" t="s">
+        <v>309</v>
+      </c>
+      <c r="F70" s="4"/>
+      <c r="G70" s="4"/>
+      <c r="H70" s="4"/>
+      <c r="I70" s="4"/>
+    </row>
+    <row r="71" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A71" s="4" t="s">
         <v>283</v>
       </c>
-      <c r="E40" s="4" t="s">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="41" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A41" t="s">
-        <v>168</v>
-      </c>
-      <c r="B41" t="s">
-        <v>169</v>
-      </c>
-      <c r="C41" t="s">
-        <v>159</v>
-      </c>
-      <c r="D41" t="s">
+      <c r="B71" s="4" t="s">
         <v>284</v>
       </c>
-      <c r="E41" s="4" t="s">
+      <c r="C71" s="4" t="s">
         <v>254</v>
       </c>
-    </row>
-    <row r="42" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A42" t="s">
-        <v>170</v>
-      </c>
-      <c r="B42" t="s">
-        <v>171</v>
-      </c>
-      <c r="C42" t="s">
-        <v>159</v>
-      </c>
-      <c r="D42" t="s">
+      <c r="D71" s="4" t="s">
+        <v>303</v>
+      </c>
+      <c r="E71" s="3" t="s">
+        <v>308</v>
+      </c>
+      <c r="F71" s="4"/>
+      <c r="G71" s="4"/>
+      <c r="H71" s="4"/>
+      <c r="I71" s="4"/>
+    </row>
+    <row r="72" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A72" s="4" t="s">
         <v>285</v>
       </c>
-      <c r="E42" s="4" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="43" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A43" s="2" t="s">
-        <v>172</v>
-      </c>
-      <c r="B43" t="s">
-        <v>173</v>
-      </c>
-      <c r="C43" t="s">
-        <v>159</v>
-      </c>
-      <c r="D43" t="s">
+      <c r="B72" s="4" t="s">
         <v>286</v>
       </c>
-      <c r="E43" s="4" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="44" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A44" t="s">
-        <v>174</v>
-      </c>
-      <c r="B44" t="s">
-        <v>175</v>
-      </c>
-      <c r="C44" t="s">
-        <v>176</v>
-      </c>
-      <c r="D44" t="s">
+      <c r="C72" s="4" t="s">
+        <v>254</v>
+      </c>
+      <c r="D72" s="4" t="s">
+        <v>304</v>
+      </c>
+      <c r="E72" s="3" t="s">
+        <v>307</v>
+      </c>
+      <c r="F72" s="4"/>
+      <c r="G72" s="4"/>
+      <c r="H72" s="4"/>
+      <c r="I72" s="4"/>
+    </row>
+    <row r="73" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A73" s="4" t="s">
         <v>287</v>
       </c>
-      <c r="E44" s="4" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="45" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A45" t="s">
-        <v>177</v>
-      </c>
-      <c r="B45" t="s">
-        <v>178</v>
-      </c>
-      <c r="C45" t="s">
-        <v>176</v>
-      </c>
-      <c r="D45" t="s">
+      <c r="B73" s="4" t="s">
         <v>288</v>
       </c>
-      <c r="E45" s="4" t="s">
-        <v>258</v>
-      </c>
-    </row>
-    <row r="46" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A46" t="s">
-        <v>179</v>
-      </c>
-      <c r="B46" t="s">
-        <v>180</v>
-      </c>
-      <c r="C46" t="s">
-        <v>176</v>
-      </c>
-      <c r="D46" t="s">
-        <v>289</v>
-      </c>
-      <c r="E46" s="4" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="47" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A47" t="s">
-        <v>181</v>
-      </c>
-      <c r="B47" t="s">
-        <v>15</v>
-      </c>
-      <c r="C47" t="s">
-        <v>176</v>
-      </c>
-      <c r="D47" t="s">
-        <v>290</v>
-      </c>
-      <c r="E47" s="4" t="s">
-        <v>260</v>
-      </c>
-    </row>
-    <row r="48" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A48" t="s">
-        <v>182</v>
-      </c>
-      <c r="B48" t="s">
-        <v>183</v>
-      </c>
-      <c r="C48" t="s">
-        <v>176</v>
-      </c>
-      <c r="D48" t="s">
-        <v>291</v>
-      </c>
-      <c r="E48" s="4" t="s">
-        <v>261</v>
-      </c>
-    </row>
-    <row r="49" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A49" t="s">
-        <v>184</v>
-      </c>
-      <c r="B49" t="s">
-        <v>185</v>
-      </c>
-      <c r="C49" t="s">
-        <v>176</v>
-      </c>
-      <c r="D49" t="s">
-        <v>292</v>
-      </c>
-      <c r="E49" s="4" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="50" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A50" t="s">
-        <v>186</v>
-      </c>
-      <c r="B50" t="s">
-        <v>31</v>
-      </c>
-      <c r="C50" t="s">
-        <v>187</v>
-      </c>
-      <c r="D50" t="s">
-        <v>293</v>
-      </c>
-      <c r="E50" s="4" t="s">
-        <v>241</v>
-      </c>
-    </row>
-    <row r="51" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A51" t="s">
-        <v>188</v>
-      </c>
-      <c r="B51" t="s">
-        <v>189</v>
-      </c>
-      <c r="C51" t="s">
-        <v>187</v>
-      </c>
-      <c r="D51" t="s">
-        <v>294</v>
-      </c>
-      <c r="E51" s="4" t="s">
-        <v>265</v>
-      </c>
-    </row>
-    <row r="52" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A52" t="s">
-        <v>190</v>
-      </c>
-      <c r="B52" t="s">
-        <v>191</v>
-      </c>
-      <c r="C52" t="s">
-        <v>187</v>
-      </c>
-      <c r="D52" t="s">
-        <v>295</v>
-      </c>
-      <c r="E52" s="4" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="53" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A53" t="s">
-        <v>192</v>
-      </c>
-      <c r="B53" t="s">
-        <v>193</v>
-      </c>
-      <c r="C53" t="s">
-        <v>187</v>
-      </c>
-      <c r="D53" t="s">
-        <v>296</v>
-      </c>
-      <c r="E53" s="4" t="s">
-        <v>264</v>
-      </c>
-    </row>
-    <row r="54" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A54" t="s">
-        <v>194</v>
-      </c>
-      <c r="B54" t="s">
-        <v>195</v>
-      </c>
-      <c r="C54" t="s">
-        <v>187</v>
-      </c>
-      <c r="D54" t="s">
-        <v>297</v>
-      </c>
-      <c r="E54" s="4" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="55" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A55" t="s">
-        <v>196</v>
-      </c>
-      <c r="B55" t="s">
-        <v>197</v>
-      </c>
-      <c r="C55" t="s">
-        <v>187</v>
-      </c>
-      <c r="D55" t="s">
-        <v>298</v>
-      </c>
-      <c r="E55" s="4" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="56" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A56" t="s">
-        <v>198</v>
-      </c>
-      <c r="B56" t="s">
-        <v>199</v>
-      </c>
-      <c r="C56" t="s">
-        <v>187</v>
-      </c>
-      <c r="D56" t="s">
-        <v>299</v>
-      </c>
-      <c r="E56" s="4" t="s">
-        <v>268</v>
-      </c>
-    </row>
-    <row r="57" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A57" t="s">
-        <v>200</v>
-      </c>
-      <c r="B57" t="s">
-        <v>201</v>
-      </c>
-      <c r="C57" t="s">
-        <v>202</v>
-      </c>
-      <c r="D57" t="s">
-        <v>300</v>
-      </c>
-      <c r="E57" s="4" t="s">
-        <v>269</v>
-      </c>
-    </row>
-    <row r="58" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A58" t="s">
-        <v>170</v>
-      </c>
-      <c r="B58" t="s">
-        <v>203</v>
-      </c>
-      <c r="C58" t="s">
-        <v>202</v>
-      </c>
-      <c r="D58" t="s">
-        <v>301</v>
-      </c>
-      <c r="E58" s="4" t="s">
-        <v>270</v>
-      </c>
-    </row>
-    <row r="59" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A59" t="s">
-        <v>204</v>
-      </c>
-      <c r="B59" t="s">
-        <v>205</v>
-      </c>
-      <c r="C59" t="s">
-        <v>202</v>
-      </c>
-      <c r="D59" t="s">
-        <v>302</v>
-      </c>
-      <c r="E59" s="4" t="s">
-        <v>271</v>
-      </c>
-    </row>
-    <row r="60" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A60" t="s">
-        <v>206</v>
-      </c>
-      <c r="B60" t="s">
-        <v>207</v>
-      </c>
-      <c r="C60" t="s">
-        <v>202</v>
-      </c>
-      <c r="D60" t="s">
-        <v>303</v>
-      </c>
-      <c r="E60" s="4" t="s">
-        <v>272</v>
-      </c>
-    </row>
-    <row r="61" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A61" t="s">
-        <v>208</v>
-      </c>
-      <c r="B61" t="s">
-        <v>209</v>
-      </c>
-      <c r="C61" t="s">
-        <v>202</v>
-      </c>
-      <c r="D61" t="s">
-        <v>304</v>
-      </c>
-      <c r="E61" s="4" t="s">
-        <v>273</v>
-      </c>
-    </row>
-    <row r="62" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A62" t="s">
-        <v>210</v>
-      </c>
-      <c r="B62" t="s">
-        <v>211</v>
-      </c>
-      <c r="C62" t="s">
-        <v>202</v>
-      </c>
-      <c r="D62" t="s">
+      <c r="C73" s="4" t="s">
+        <v>254</v>
+      </c>
+      <c r="D73" s="4" t="s">
         <v>305</v>
       </c>
-      <c r="E62" s="4" t="s">
-        <v>274</v>
-      </c>
-    </row>
-    <row r="63" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A63" t="s">
-        <v>168</v>
-      </c>
-      <c r="B63" t="s">
-        <v>212</v>
-      </c>
-      <c r="C63" t="s">
-        <v>202</v>
-      </c>
-      <c r="D63" t="s">
+      <c r="E73" s="3" t="s">
         <v>306</v>
       </c>
-      <c r="E63" s="4" t="s">
-        <v>275</v>
-      </c>
-    </row>
-    <row r="64" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A64" t="s">
-        <v>213</v>
-      </c>
-      <c r="B64" t="s">
-        <v>214</v>
-      </c>
-      <c r="C64" t="s">
-        <v>202</v>
-      </c>
-      <c r="D64" t="s">
-        <v>307</v>
-      </c>
-      <c r="E64" s="4" t="s">
-        <v>276</v>
-      </c>
-    </row>
-    <row r="65" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A65" t="s">
-        <v>215</v>
-      </c>
-      <c r="B65" t="s">
-        <v>216</v>
-      </c>
-      <c r="C65" t="s">
-        <v>202</v>
-      </c>
-      <c r="D65" t="s">
-        <v>308</v>
-      </c>
-      <c r="E65" s="4" t="s">
-        <v>277</v>
-      </c>
-    </row>
-    <row r="66" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A66" t="s">
-        <v>217</v>
-      </c>
-      <c r="B66" t="s">
-        <v>218</v>
-      </c>
-      <c r="C66" t="s">
-        <v>202</v>
-      </c>
-      <c r="D66" t="s">
-        <v>309</v>
-      </c>
-      <c r="E66" s="4" t="s">
-        <v>278</v>
-      </c>
-    </row>
-    <row r="67" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A67" t="s">
-        <v>219</v>
-      </c>
-      <c r="B67" t="s">
-        <v>220</v>
-      </c>
-      <c r="C67" t="s">
-        <v>202</v>
-      </c>
-      <c r="D67" t="s">
-        <v>310</v>
-      </c>
-      <c r="E67" s="4" t="s">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="68" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A68" t="s">
-        <v>164</v>
-      </c>
-      <c r="B68" t="s">
-        <v>221</v>
-      </c>
-      <c r="C68" t="s">
-        <v>202</v>
-      </c>
-      <c r="D68" t="s">
-        <v>311</v>
-      </c>
-      <c r="E68" s="4" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="69" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A69" t="s">
-        <v>222</v>
-      </c>
-      <c r="B69" t="s">
-        <v>223</v>
-      </c>
-      <c r="C69" t="s">
-        <v>202</v>
-      </c>
-      <c r="D69" t="s">
-        <v>312</v>
-      </c>
-      <c r="E69" s="4" t="s">
-        <v>249</v>
-      </c>
-    </row>
-    <row r="70" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A70" t="s">
-        <v>162</v>
-      </c>
-      <c r="B70" t="s">
-        <v>224</v>
-      </c>
-      <c r="C70" t="s">
-        <v>202</v>
-      </c>
-      <c r="D70" t="s">
-        <v>313</v>
-      </c>
-      <c r="E70" s="4" t="s">
-        <v>248</v>
-      </c>
-    </row>
-    <row r="71" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A71" t="s">
-        <v>225</v>
-      </c>
-      <c r="B71" t="s">
-        <v>226</v>
-      </c>
-      <c r="C71" t="s">
-        <v>202</v>
-      </c>
-      <c r="D71" t="s">
-        <v>314</v>
-      </c>
-      <c r="E71" s="4" t="s">
-        <v>247</v>
-      </c>
-    </row>
-    <row r="72" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A72" t="s">
-        <v>227</v>
-      </c>
-      <c r="B72" t="s">
-        <v>228</v>
-      </c>
-      <c r="C72" t="s">
-        <v>202</v>
-      </c>
-      <c r="D72" t="s">
-        <v>315</v>
-      </c>
-      <c r="E72" s="4" t="s">
-        <v>246</v>
-      </c>
-    </row>
-    <row r="73" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A73" t="s">
-        <v>229</v>
-      </c>
-      <c r="B73" t="s">
-        <v>230</v>
-      </c>
-      <c r="C73" t="s">
-        <v>202</v>
-      </c>
-      <c r="D73" t="s">
-        <v>316</v>
-      </c>
-      <c r="E73" s="4" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="74" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="75" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="76" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="77" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="78" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="79" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="80" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+      <c r="F73" s="4"/>
+      <c r="G73" s="4"/>
+      <c r="H73" s="4"/>
+      <c r="I73" s="4"/>
+    </row>
+    <row r="74" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="75" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="76" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="77" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="78" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="79" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="80" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
     <row r="81" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
     <row r="82" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
     <row r="83" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
Fixed most sound issues
</commit_message>
<xml_diff>
--- a/hmoob_lus/PDF HLLA.xlsx
+++ b/hmoob_lus/PDF HLLA.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ntxhw\Desktop\Projects\HLLA\hmoob_lus\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E87FCBFE-8B23-4CE2-95A5-79C7417E8168}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9456D276-8047-4410-A3F0-2D4297FBA04A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="391" uniqueCount="317">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="402" uniqueCount="317">
   <si>
     <t>English Word</t>
   </si>
@@ -715,9 +715,6 @@
     <t>Male - Double Vowel AU.wav</t>
   </si>
   <si>
-    <t>Female - Double  Vowel AU.wav</t>
-  </si>
-  <si>
     <t>aw</t>
   </si>
   <si>
@@ -727,9 +724,6 @@
     <t>Male - Double Vowel AW.wav</t>
   </si>
   <si>
-    <t>Female - Double  Vowel AW.wav</t>
-  </si>
-  <si>
     <t>ee</t>
   </si>
   <si>
@@ -739,9 +733,6 @@
     <t>Male - Double Vowel EE.wav</t>
   </si>
   <si>
-    <t>Female - Double  Vowel EE.wav</t>
-  </si>
-  <si>
     <t>ia</t>
   </si>
   <si>
@@ -751,9 +742,6 @@
     <t>Male - Double Vowel IA.wav</t>
   </si>
   <si>
-    <t>Female - Double  Vowel IA.wav</t>
-  </si>
-  <si>
     <t>oo</t>
   </si>
   <si>
@@ -763,9 +751,6 @@
     <t>Male - Double Vowel OO.wav</t>
   </si>
   <si>
-    <t>Female - Double  Vowel OO.wav</t>
-  </si>
-  <si>
     <t>ua</t>
   </si>
   <si>
@@ -775,9 +760,6 @@
     <t>Male - Double Vowel UA.wav</t>
   </si>
   <si>
-    <t>Female - Double  Vowel UA.wav</t>
-  </si>
-  <si>
     <t>c</t>
   </si>
   <si>
@@ -790,9 +772,6 @@
     <t>dos dev</t>
   </si>
   <si>
-    <t>Female - Consonant D.wav</t>
-  </si>
-  <si>
     <t>f</t>
   </si>
   <si>
@@ -805,9 +784,6 @@
     <t>hos haus</t>
   </si>
   <si>
-    <t>Female - Consonant H.wav</t>
-  </si>
-  <si>
     <t>k</t>
   </si>
   <si>
@@ -820,9 +796,6 @@
     <t>los liab</t>
   </si>
   <si>
-    <t>Female - Consonant L.wav</t>
-  </si>
-  <si>
     <t>mos miv</t>
   </si>
   <si>
@@ -832,9 +805,6 @@
     <t>nos noog</t>
   </si>
   <si>
-    <t>Female - Consonant N.wav</t>
-  </si>
-  <si>
     <t>p</t>
   </si>
   <si>
@@ -847,9 +817,6 @@
     <t xml:space="preserve">qos qav </t>
   </si>
   <si>
-    <t>Female - Consonant Q.wav</t>
-  </si>
-  <si>
     <t>r</t>
   </si>
   <si>
@@ -865,9 +832,6 @@
     <t>tos twm</t>
   </si>
   <si>
-    <t>Female - Consonant T.wav</t>
-  </si>
-  <si>
     <t>vos vas</t>
   </si>
   <si>
@@ -971,6 +935,42 @@
   </si>
   <si>
     <t>Female - Single Consonant C.wav</t>
+  </si>
+  <si>
+    <t>Female - Single Consonant T.wav</t>
+  </si>
+  <si>
+    <t>Female - Single Consonant Q.wav</t>
+  </si>
+  <si>
+    <t>Female - Single Consonant N.wav</t>
+  </si>
+  <si>
+    <t>Female - Single Consonant L.wav</t>
+  </si>
+  <si>
+    <t>Female - Single Consonant D.wav</t>
+  </si>
+  <si>
+    <t>Female - Single Consonant H.wav</t>
+  </si>
+  <si>
+    <t>Female - Double Vowel AU.wav</t>
+  </si>
+  <si>
+    <t>Female - Double Vowel AW.wav</t>
+  </si>
+  <si>
+    <t>Female - Double Vowel EE.wav</t>
+  </si>
+  <si>
+    <t>Female - Double Vowel IA.wav</t>
+  </si>
+  <si>
+    <t>Female - Double Vowel OO.wav</t>
+  </si>
+  <si>
+    <t>Female - Double Vowel UA.wav</t>
   </si>
 </sst>
 </file>
@@ -1387,8 +1387,8 @@
   </sheetPr>
   <dimension ref="A1:J1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="A57" sqref="A57"/>
+    <sheetView tabSelected="1" topLeftCell="B62" workbookViewId="0">
+      <selection activeCell="E61" sqref="E61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2522,7 +2522,7 @@
         <v>230</v>
       </c>
       <c r="E51" s="3" t="s">
-        <v>231</v>
+        <v>311</v>
       </c>
       <c r="F51" s="4"/>
       <c r="G51" s="4"/>
@@ -2531,19 +2531,19 @@
     </row>
     <row r="52" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A52" s="4" t="s">
+        <v>231</v>
+      </c>
+      <c r="B52" s="4" t="s">
         <v>232</v>
-      </c>
-      <c r="B52" s="4" t="s">
-        <v>233</v>
       </c>
       <c r="C52" s="4" t="s">
         <v>225</v>
       </c>
       <c r="D52" s="4" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="E52" s="3" t="s">
-        <v>235</v>
+        <v>312</v>
       </c>
       <c r="F52" s="4"/>
       <c r="G52" s="4"/>
@@ -2552,19 +2552,19 @@
     </row>
     <row r="53" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A53" s="4" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="B53" s="4" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="C53" s="4" t="s">
         <v>225</v>
       </c>
       <c r="D53" s="4" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="E53" s="3" t="s">
-        <v>239</v>
+        <v>313</v>
       </c>
       <c r="F53" s="4"/>
       <c r="G53" s="4"/>
@@ -2573,19 +2573,19 @@
     </row>
     <row r="54" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A54" s="4" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
       <c r="B54" s="4" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
       <c r="C54" s="4" t="s">
         <v>225</v>
       </c>
       <c r="D54" s="4" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="E54" s="3" t="s">
-        <v>243</v>
+        <v>314</v>
       </c>
       <c r="F54" s="4"/>
       <c r="G54" s="4"/>
@@ -2594,19 +2594,19 @@
     </row>
     <row r="55" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A55" s="4" t="s">
-        <v>244</v>
+        <v>240</v>
       </c>
       <c r="B55" s="4" t="s">
-        <v>245</v>
+        <v>241</v>
       </c>
       <c r="C55" s="4" t="s">
         <v>225</v>
       </c>
       <c r="D55" s="4" t="s">
-        <v>246</v>
+        <v>242</v>
       </c>
       <c r="E55" s="3" t="s">
-        <v>247</v>
+        <v>315</v>
       </c>
       <c r="F55" s="4"/>
       <c r="G55" s="4"/>
@@ -2615,19 +2615,19 @@
     </row>
     <row r="56" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A56" s="4" t="s">
-        <v>248</v>
+        <v>243</v>
       </c>
       <c r="B56" s="4" t="s">
-        <v>249</v>
+        <v>244</v>
       </c>
       <c r="C56" s="4" t="s">
         <v>225</v>
       </c>
       <c r="D56" s="4" t="s">
-        <v>250</v>
+        <v>245</v>
       </c>
       <c r="E56" s="3" t="s">
-        <v>251</v>
+        <v>316</v>
       </c>
       <c r="F56" s="4"/>
       <c r="G56" s="4"/>
@@ -2636,21 +2636,23 @@
     </row>
     <row r="57" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A57" s="4" t="s">
-        <v>252</v>
+        <v>246</v>
       </c>
       <c r="B57" s="4" t="s">
-        <v>253</v>
+        <v>247</v>
       </c>
       <c r="C57" s="4" t="s">
-        <v>254</v>
+        <v>248</v>
       </c>
       <c r="D57" s="4" t="s">
-        <v>290</v>
+        <v>278</v>
       </c>
       <c r="E57" s="3" t="s">
-        <v>316</v>
-      </c>
-      <c r="F57" s="4"/>
+        <v>304</v>
+      </c>
+      <c r="F57" s="4" t="s">
+        <v>273</v>
+      </c>
       <c r="G57" s="4"/>
       <c r="H57" s="4"/>
       <c r="I57" s="4"/>
@@ -2660,16 +2662,16 @@
         <v>192</v>
       </c>
       <c r="B58" s="4" t="s">
-        <v>255</v>
+        <v>249</v>
       </c>
       <c r="C58" s="4" t="s">
-        <v>254</v>
+        <v>248</v>
       </c>
       <c r="D58" s="4" t="s">
-        <v>291</v>
+        <v>279</v>
       </c>
       <c r="E58" s="3" t="s">
-        <v>256</v>
+        <v>309</v>
       </c>
       <c r="F58" s="4"/>
       <c r="G58" s="4"/>
@@ -2678,40 +2680,42 @@
     </row>
     <row r="59" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A59" s="4" t="s">
-        <v>257</v>
+        <v>250</v>
       </c>
       <c r="B59" s="4" t="s">
-        <v>258</v>
+        <v>251</v>
       </c>
       <c r="C59" s="4" t="s">
-        <v>254</v>
+        <v>248</v>
       </c>
       <c r="D59" s="4" t="s">
-        <v>292</v>
+        <v>280</v>
       </c>
       <c r="E59" s="3" t="s">
-        <v>315</v>
-      </c>
-      <c r="F59" s="4"/>
+        <v>303</v>
+      </c>
+      <c r="F59" s="4" t="s">
+        <v>273</v>
+      </c>
       <c r="G59" s="4"/>
       <c r="H59" s="4"/>
       <c r="I59" s="4"/>
     </row>
     <row r="60" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A60" s="4" t="s">
-        <v>259</v>
+        <v>252</v>
       </c>
       <c r="B60" s="4" t="s">
-        <v>260</v>
+        <v>253</v>
       </c>
       <c r="C60" s="4" t="s">
-        <v>254</v>
+        <v>248</v>
       </c>
       <c r="D60" s="4" t="s">
-        <v>293</v>
+        <v>281</v>
       </c>
       <c r="E60" s="3" t="s">
-        <v>261</v>
+        <v>310</v>
       </c>
       <c r="F60" s="4"/>
       <c r="G60" s="4"/>
@@ -2720,40 +2724,42 @@
     </row>
     <row r="61" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A61" s="4" t="s">
-        <v>262</v>
+        <v>254</v>
       </c>
       <c r="B61" s="4" t="s">
-        <v>263</v>
+        <v>255</v>
       </c>
       <c r="C61" s="4" t="s">
-        <v>254</v>
+        <v>248</v>
       </c>
       <c r="D61" s="4" t="s">
-        <v>294</v>
+        <v>282</v>
       </c>
       <c r="E61" s="3" t="s">
-        <v>314</v>
-      </c>
-      <c r="F61" s="4"/>
+        <v>302</v>
+      </c>
+      <c r="F61" s="4" t="s">
+        <v>273</v>
+      </c>
       <c r="G61" s="4"/>
       <c r="H61" s="4"/>
       <c r="I61" s="4"/>
     </row>
     <row r="62" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A62" s="4" t="s">
-        <v>264</v>
+        <v>256</v>
       </c>
       <c r="B62" s="4" t="s">
-        <v>265</v>
+        <v>257</v>
       </c>
       <c r="C62" s="4" t="s">
-        <v>254</v>
+        <v>248</v>
       </c>
       <c r="D62" s="4" t="s">
-        <v>289</v>
+        <v>277</v>
       </c>
       <c r="E62" s="3" t="s">
-        <v>266</v>
+        <v>308</v>
       </c>
       <c r="F62" s="4"/>
       <c r="G62" s="4"/>
@@ -2765,37 +2771,39 @@
         <v>188</v>
       </c>
       <c r="B63" s="4" t="s">
-        <v>267</v>
+        <v>258</v>
       </c>
       <c r="C63" s="4" t="s">
-        <v>254</v>
+        <v>248</v>
       </c>
       <c r="D63" s="4" t="s">
-        <v>295</v>
+        <v>283</v>
       </c>
       <c r="E63" s="3" t="s">
-        <v>313</v>
-      </c>
-      <c r="F63" s="4"/>
+        <v>301</v>
+      </c>
+      <c r="F63" s="4" t="s">
+        <v>273</v>
+      </c>
       <c r="G63" s="4"/>
       <c r="H63" s="4"/>
       <c r="I63" s="4"/>
     </row>
     <row r="64" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A64" s="4" t="s">
-        <v>268</v>
+        <v>259</v>
       </c>
       <c r="B64" s="4" t="s">
-        <v>269</v>
+        <v>260</v>
       </c>
       <c r="C64" s="4" t="s">
-        <v>254</v>
+        <v>248</v>
       </c>
       <c r="D64" s="4" t="s">
-        <v>296</v>
+        <v>284</v>
       </c>
       <c r="E64" s="3" t="s">
-        <v>270</v>
+        <v>307</v>
       </c>
       <c r="F64" s="4"/>
       <c r="G64" s="4"/>
@@ -2804,40 +2812,42 @@
     </row>
     <row r="65" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A65" s="4" t="s">
-        <v>271</v>
+        <v>261</v>
       </c>
       <c r="B65" s="4" t="s">
-        <v>272</v>
+        <v>262</v>
       </c>
       <c r="C65" s="4" t="s">
-        <v>254</v>
+        <v>248</v>
       </c>
       <c r="D65" s="4" t="s">
-        <v>297</v>
+        <v>285</v>
       </c>
       <c r="E65" s="3" t="s">
-        <v>312</v>
-      </c>
-      <c r="F65" s="4"/>
+        <v>300</v>
+      </c>
+      <c r="F65" s="4" t="s">
+        <v>273</v>
+      </c>
       <c r="G65" s="4"/>
       <c r="H65" s="4"/>
       <c r="I65" s="4"/>
     </row>
     <row r="66" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A66" s="4" t="s">
-        <v>273</v>
+        <v>263</v>
       </c>
       <c r="B66" s="4" t="s">
-        <v>274</v>
+        <v>264</v>
       </c>
       <c r="C66" s="4" t="s">
-        <v>254</v>
+        <v>248</v>
       </c>
       <c r="D66" s="4" t="s">
-        <v>298</v>
+        <v>286</v>
       </c>
       <c r="E66" s="3" t="s">
-        <v>275</v>
+        <v>306</v>
       </c>
       <c r="F66" s="4"/>
       <c r="G66" s="4"/>
@@ -2846,21 +2856,23 @@
     </row>
     <row r="67" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A67" s="4" t="s">
-        <v>276</v>
+        <v>265</v>
       </c>
       <c r="B67" s="4" t="s">
-        <v>277</v>
+        <v>266</v>
       </c>
       <c r="C67" s="4" t="s">
-        <v>254</v>
+        <v>248</v>
       </c>
       <c r="D67" s="4" t="s">
+        <v>287</v>
+      </c>
+      <c r="E67" s="3" t="s">
         <v>299</v>
       </c>
-      <c r="E67" s="3" t="s">
-        <v>311</v>
-      </c>
-      <c r="F67" s="4"/>
+      <c r="F67" s="4" t="s">
+        <v>273</v>
+      </c>
       <c r="G67" s="4"/>
       <c r="H67" s="4"/>
       <c r="I67" s="4"/>
@@ -2870,37 +2882,39 @@
         <v>180</v>
       </c>
       <c r="B68" s="4" t="s">
-        <v>278</v>
+        <v>267</v>
       </c>
       <c r="C68" s="4" t="s">
-        <v>254</v>
+        <v>248</v>
       </c>
       <c r="D68" s="4" t="s">
-        <v>300</v>
+        <v>288</v>
       </c>
       <c r="E68" s="3" t="s">
-        <v>310</v>
-      </c>
-      <c r="F68" s="4"/>
+        <v>298</v>
+      </c>
+      <c r="F68" s="4" t="s">
+        <v>273</v>
+      </c>
       <c r="G68" s="4"/>
       <c r="H68" s="4"/>
       <c r="I68" s="4"/>
     </row>
     <row r="69" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A69" s="4" t="s">
-        <v>279</v>
+        <v>268</v>
       </c>
       <c r="B69" s="4" t="s">
-        <v>280</v>
+        <v>269</v>
       </c>
       <c r="C69" s="4" t="s">
-        <v>254</v>
+        <v>248</v>
       </c>
       <c r="D69" s="4" t="s">
-        <v>301</v>
+        <v>289</v>
       </c>
       <c r="E69" s="3" t="s">
-        <v>281</v>
+        <v>305</v>
       </c>
       <c r="F69" s="4"/>
       <c r="G69" s="4"/>
@@ -2912,86 +2926,96 @@
         <v>176</v>
       </c>
       <c r="B70" s="4" t="s">
-        <v>282</v>
+        <v>270</v>
       </c>
       <c r="C70" s="4" t="s">
-        <v>254</v>
+        <v>248</v>
       </c>
       <c r="D70" s="4" t="s">
-        <v>302</v>
+        <v>290</v>
       </c>
       <c r="E70" s="3" t="s">
-        <v>309</v>
-      </c>
-      <c r="F70" s="4"/>
+        <v>297</v>
+      </c>
+      <c r="F70" s="4" t="s">
+        <v>273</v>
+      </c>
       <c r="G70" s="4"/>
       <c r="H70" s="4"/>
       <c r="I70" s="4"/>
     </row>
     <row r="71" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A71" s="4" t="s">
-        <v>283</v>
+        <v>271</v>
       </c>
       <c r="B71" s="4" t="s">
-        <v>284</v>
+        <v>272</v>
       </c>
       <c r="C71" s="4" t="s">
-        <v>254</v>
+        <v>248</v>
       </c>
       <c r="D71" s="4" t="s">
-        <v>303</v>
+        <v>291</v>
       </c>
       <c r="E71" s="3" t="s">
-        <v>308</v>
-      </c>
-      <c r="F71" s="4"/>
+        <v>296</v>
+      </c>
+      <c r="F71" s="4" t="s">
+        <v>273</v>
+      </c>
       <c r="G71" s="4"/>
       <c r="H71" s="4"/>
       <c r="I71" s="4"/>
     </row>
     <row r="72" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A72" s="4" t="s">
-        <v>285</v>
+        <v>273</v>
       </c>
       <c r="B72" s="4" t="s">
-        <v>286</v>
+        <v>274</v>
       </c>
       <c r="C72" s="4" t="s">
-        <v>254</v>
+        <v>248</v>
       </c>
       <c r="D72" s="4" t="s">
-        <v>304</v>
+        <v>292</v>
       </c>
       <c r="E72" s="3" t="s">
-        <v>307</v>
-      </c>
-      <c r="F72" s="4"/>
+        <v>295</v>
+      </c>
+      <c r="F72" s="4" t="s">
+        <v>273</v>
+      </c>
       <c r="G72" s="4"/>
       <c r="H72" s="4"/>
       <c r="I72" s="4"/>
     </row>
     <row r="73" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A73" s="4" t="s">
-        <v>287</v>
+        <v>275</v>
       </c>
       <c r="B73" s="4" t="s">
-        <v>288</v>
+        <v>276</v>
       </c>
       <c r="C73" s="4" t="s">
-        <v>254</v>
+        <v>248</v>
       </c>
       <c r="D73" s="4" t="s">
-        <v>305</v>
+        <v>293</v>
       </c>
       <c r="E73" s="3" t="s">
-        <v>306</v>
-      </c>
-      <c r="F73" s="4"/>
+        <v>294</v>
+      </c>
+      <c r="F73" s="4" t="s">
+        <v>273</v>
+      </c>
       <c r="G73" s="4"/>
       <c r="H73" s="4"/>
       <c r="I73" s="4"/>
     </row>
-    <row r="74" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="74" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="C74" s="4"/>
+    </row>
     <row r="75" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
     <row r="76" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
     <row r="77" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
modified audio cim kuv
</commit_message>
<xml_diff>
--- a/hmoob_lus/PDF HLLA.xlsx
+++ b/hmoob_lus/PDF HLLA.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ntxhw\Desktop\Projects\HLLA\hmoob_lus\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9456D276-8047-4410-A3F0-2D4297FBA04A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE1B64B0-04FE-4946-BC5C-FE1C4EB8882C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1387,8 +1387,8 @@
   </sheetPr>
   <dimension ref="A1:J1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B62" workbookViewId="0">
-      <selection activeCell="E61" sqref="E61"/>
+    <sheetView tabSelected="1" topLeftCell="A30" workbookViewId="0">
+      <selection activeCell="E38" sqref="E38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>